<commit_message>
Update edited session - 2025-10-11T09:36:52.090Z - Cache Bust ID: 1760175412090m01lh0p3c
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_General_Surgery_scanner1760170816881_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
+++ b/log_history/Y4_B2526_General_Surgery_scanner1760170816881_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Scanner" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F116"/>
+  <dimension ref="A1:F115"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -704,7 +704,7 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>200359</v>
+        <v>200877</v>
       </c>
       <c r="B16" t="str">
         <v>General Surgery</v>
@@ -713,7 +713,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D16" t="str">
-        <v>11:24:35</v>
+        <v>11:24:44</v>
       </c>
       <c r="E16" t="str">
         <v>Manual</v>
@@ -724,7 +724,7 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>200877</v>
+        <v>191480</v>
       </c>
       <c r="B17" t="str">
         <v>General Surgery</v>
@@ -733,7 +733,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D17" t="str">
-        <v>11:24:44</v>
+        <v>11:24:53</v>
       </c>
       <c r="E17" t="str">
         <v>Manual</v>
@@ -744,7 +744,7 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>191480</v>
+        <v>191375</v>
       </c>
       <c r="B18" t="str">
         <v>General Surgery</v>
@@ -753,7 +753,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D18" t="str">
-        <v>11:24:53</v>
+        <v>11:25:26</v>
       </c>
       <c r="E18" t="str">
         <v>Manual</v>
@@ -764,7 +764,7 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>191375</v>
+        <v>201218</v>
       </c>
       <c r="B19" t="str">
         <v>General Surgery</v>
@@ -773,7 +773,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D19" t="str">
-        <v>11:25:26</v>
+        <v>11:25:32</v>
       </c>
       <c r="E19" t="str">
         <v>Manual</v>
@@ -784,7 +784,7 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>201218</v>
+        <v>201438</v>
       </c>
       <c r="B20" t="str">
         <v>General Surgery</v>
@@ -793,7 +793,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D20" t="str">
-        <v>11:25:32</v>
+        <v>11:25:50</v>
       </c>
       <c r="E20" t="str">
         <v>Manual</v>
@@ -804,7 +804,7 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>201438</v>
+        <v>191186</v>
       </c>
       <c r="B21" t="str">
         <v>General Surgery</v>
@@ -813,7 +813,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D21" t="str">
-        <v>11:25:50</v>
+        <v>11:26:11</v>
       </c>
       <c r="E21" t="str">
         <v>Manual</v>
@@ -824,7 +824,7 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>191186</v>
+        <v>191258</v>
       </c>
       <c r="B22" t="str">
         <v>General Surgery</v>
@@ -833,7 +833,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D22" t="str">
-        <v>11:26:11</v>
+        <v>11:27:36</v>
       </c>
       <c r="E22" t="str">
         <v>Manual</v>
@@ -844,7 +844,7 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>191258</v>
+        <v>200742</v>
       </c>
       <c r="B23" t="str">
         <v>General Surgery</v>
@@ -853,7 +853,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D23" t="str">
-        <v>11:27:36</v>
+        <v>11:27:56</v>
       </c>
       <c r="E23" t="str">
         <v>Manual</v>
@@ -864,7 +864,7 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>200742</v>
+        <v>201563</v>
       </c>
       <c r="B24" t="str">
         <v>General Surgery</v>
@@ -873,7 +873,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D24" t="str">
-        <v>11:27:56</v>
+        <v>11:28:13</v>
       </c>
       <c r="E24" t="str">
         <v>Manual</v>
@@ -884,7 +884,7 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>201563</v>
+        <v>180804</v>
       </c>
       <c r="B25" t="str">
         <v>General Surgery</v>
@@ -893,7 +893,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D25" t="str">
-        <v>11:28:13</v>
+        <v>11:28:23</v>
       </c>
       <c r="E25" t="str">
         <v>Manual</v>
@@ -904,7 +904,7 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>180804</v>
+        <v>211167</v>
       </c>
       <c r="B26" t="str">
         <v>General Surgery</v>
@@ -913,7 +913,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D26" t="str">
-        <v>11:28:23</v>
+        <v>11:28:31</v>
       </c>
       <c r="E26" t="str">
         <v>Manual</v>
@@ -924,7 +924,7 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>211167</v>
+        <v>211169</v>
       </c>
       <c r="B27" t="str">
         <v>General Surgery</v>
@@ -933,7 +933,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D27" t="str">
-        <v>11:28:31</v>
+        <v>11:28:41</v>
       </c>
       <c r="E27" t="str">
         <v>Manual</v>
@@ -944,7 +944,7 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>211169</v>
+        <v>211079</v>
       </c>
       <c r="B28" t="str">
         <v>General Surgery</v>
@@ -953,7 +953,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D28" t="str">
-        <v>11:28:41</v>
+        <v>11:28:48</v>
       </c>
       <c r="E28" t="str">
         <v>Manual</v>
@@ -964,7 +964,7 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>211079</v>
+        <v>200468</v>
       </c>
       <c r="B29" t="str">
         <v>General Surgery</v>
@@ -973,7 +973,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D29" t="str">
-        <v>11:28:48</v>
+        <v>11:29:01</v>
       </c>
       <c r="E29" t="str">
         <v>Manual</v>
@@ -984,7 +984,7 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>200468</v>
+        <v>191109</v>
       </c>
       <c r="B30" t="str">
         <v>General Surgery</v>
@@ -993,7 +993,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D30" t="str">
-        <v>11:29:01</v>
+        <v>11:29:08</v>
       </c>
       <c r="E30" t="str">
         <v>Manual</v>
@@ -1004,7 +1004,7 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>191109</v>
+        <v>191088</v>
       </c>
       <c r="B31" t="str">
         <v>General Surgery</v>
@@ -1013,7 +1013,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D31" t="str">
-        <v>11:29:08</v>
+        <v>11:29:17</v>
       </c>
       <c r="E31" t="str">
         <v>Manual</v>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>191088</v>
+        <v>200423</v>
       </c>
       <c r="B32" t="str">
         <v>General Surgery</v>
@@ -1033,7 +1033,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D32" t="str">
-        <v>11:29:17</v>
+        <v>11:29:25</v>
       </c>
       <c r="E32" t="str">
         <v>Manual</v>
@@ -1044,7 +1044,7 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>200423</v>
+        <v>190931</v>
       </c>
       <c r="B33" t="str">
         <v>General Surgery</v>
@@ -1053,7 +1053,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D33" t="str">
-        <v>11:29:25</v>
+        <v>11:29:35</v>
       </c>
       <c r="E33" t="str">
         <v>Manual</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>190931</v>
+        <v>190922</v>
       </c>
       <c r="B34" t="str">
         <v>General Surgery</v>
@@ -1073,7 +1073,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D34" t="str">
-        <v>11:29:35</v>
+        <v>11:29:50</v>
       </c>
       <c r="E34" t="str">
         <v>Manual</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>190922</v>
+        <v>191131</v>
       </c>
       <c r="B35" t="str">
         <v>General Surgery</v>
@@ -1093,7 +1093,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D35" t="str">
-        <v>11:29:50</v>
+        <v>11:30:02</v>
       </c>
       <c r="E35" t="str">
         <v>Manual</v>
@@ -1104,7 +1104,7 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>191131</v>
+        <v>190803</v>
       </c>
       <c r="B36" t="str">
         <v>General Surgery</v>
@@ -1113,7 +1113,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D36" t="str">
-        <v>11:30:02</v>
+        <v>11:30:15</v>
       </c>
       <c r="E36" t="str">
         <v>Manual</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>190803</v>
+        <v>181013</v>
       </c>
       <c r="B37" t="str">
         <v>General Surgery</v>
@@ -1133,7 +1133,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D37" t="str">
-        <v>11:30:15</v>
+        <v>11:30:22</v>
       </c>
       <c r="E37" t="str">
         <v>Manual</v>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>181013</v>
+        <v>201495</v>
       </c>
       <c r="B38" t="str">
         <v>General Surgery</v>
@@ -1153,7 +1153,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D38" t="str">
-        <v>11:30:22</v>
+        <v>11:30:50</v>
       </c>
       <c r="E38" t="str">
         <v>Manual</v>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>201495</v>
+        <v>201026</v>
       </c>
       <c r="B39" t="str">
         <v>General Surgery</v>
@@ -1173,7 +1173,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D39" t="str">
-        <v>11:30:50</v>
+        <v>11:33:15</v>
       </c>
       <c r="E39" t="str">
         <v>Manual</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>201026</v>
+        <v>200850</v>
       </c>
       <c r="B40" t="str">
         <v>General Surgery</v>
@@ -1193,7 +1193,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D40" t="str">
-        <v>11:33:15</v>
+        <v>11:33:26</v>
       </c>
       <c r="E40" t="str">
         <v>Manual</v>
@@ -1204,7 +1204,7 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>200850</v>
+        <v>200866</v>
       </c>
       <c r="B41" t="str">
         <v>General Surgery</v>
@@ -1213,7 +1213,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D41" t="str">
-        <v>11:33:26</v>
+        <v>11:33:36</v>
       </c>
       <c r="E41" t="str">
         <v>Manual</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>200866</v>
+        <v>201834</v>
       </c>
       <c r="B42" t="str">
         <v>General Surgery</v>
@@ -1233,7 +1233,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D42" t="str">
-        <v>11:33:36</v>
+        <v>11:35:22</v>
       </c>
       <c r="E42" t="str">
         <v>Manual</v>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>201834</v>
+        <v>211118</v>
       </c>
       <c r="B43" t="str">
         <v>General Surgery</v>
@@ -1253,7 +1253,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D43" t="str">
-        <v>11:35:22</v>
+        <v>11:36:25</v>
       </c>
       <c r="E43" t="str">
         <v>Manual</v>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>211118</v>
+        <v>200904</v>
       </c>
       <c r="B44" t="str">
         <v>General Surgery</v>
@@ -1273,7 +1273,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D44" t="str">
-        <v>11:36:25</v>
+        <v>11:37:01</v>
       </c>
       <c r="E44" t="str">
         <v>Manual</v>
@@ -1284,7 +1284,7 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>200904</v>
+        <v>201632</v>
       </c>
       <c r="B45" t="str">
         <v>General Surgery</v>
@@ -1293,7 +1293,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D45" t="str">
-        <v>11:37:01</v>
+        <v>11:37:08</v>
       </c>
       <c r="E45" t="str">
         <v>Manual</v>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>201632</v>
+        <v>201190</v>
       </c>
       <c r="B46" t="str">
         <v>General Surgery</v>
@@ -1313,7 +1313,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D46" t="str">
-        <v>11:37:08</v>
+        <v>11:37:15</v>
       </c>
       <c r="E46" t="str">
         <v>Manual</v>
@@ -1324,7 +1324,7 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>201190</v>
+        <v>200824</v>
       </c>
       <c r="B47" t="str">
         <v>General Surgery</v>
@@ -1333,7 +1333,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D47" t="str">
-        <v>11:37:15</v>
+        <v>11:37:21</v>
       </c>
       <c r="E47" t="str">
         <v>Manual</v>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>200824</v>
+        <v>201197</v>
       </c>
       <c r="B48" t="str">
         <v>General Surgery</v>
@@ -1353,7 +1353,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D48" t="str">
-        <v>11:37:21</v>
+        <v>11:37:28</v>
       </c>
       <c r="E48" t="str">
         <v>Manual</v>
@@ -1364,7 +1364,7 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>201197</v>
+        <v>200914</v>
       </c>
       <c r="B49" t="str">
         <v>General Surgery</v>
@@ -1373,7 +1373,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D49" t="str">
-        <v>11:37:28</v>
+        <v>11:37:39</v>
       </c>
       <c r="E49" t="str">
         <v>Manual</v>
@@ -1384,7 +1384,7 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>200914</v>
+        <v>201065</v>
       </c>
       <c r="B50" t="str">
         <v>General Surgery</v>
@@ -1393,7 +1393,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D50" t="str">
-        <v>11:37:39</v>
+        <v>11:38:11</v>
       </c>
       <c r="E50" t="str">
         <v>Manual</v>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>201065</v>
+        <v>191478</v>
       </c>
       <c r="B51" t="str">
         <v>General Surgery</v>
@@ -1413,7 +1413,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D51" t="str">
-        <v>11:38:11</v>
+        <v>11:38:32</v>
       </c>
       <c r="E51" t="str">
         <v>Manual</v>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>191478</v>
+        <v>200999</v>
       </c>
       <c r="B52" t="str">
         <v>General Surgery</v>
@@ -1433,7 +1433,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D52" t="str">
-        <v>11:38:32</v>
+        <v>11:38:40</v>
       </c>
       <c r="E52" t="str">
         <v>Manual</v>
@@ -1444,7 +1444,7 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>200999</v>
+        <v>201157</v>
       </c>
       <c r="B53" t="str">
         <v>General Surgery</v>
@@ -1453,7 +1453,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D53" t="str">
-        <v>11:38:40</v>
+        <v>11:38:51</v>
       </c>
       <c r="E53" t="str">
         <v>Manual</v>
@@ -1464,7 +1464,7 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>201157</v>
+        <v>190314</v>
       </c>
       <c r="B54" t="str">
         <v>General Surgery</v>
@@ -1473,7 +1473,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D54" t="str">
-        <v>11:38:51</v>
+        <v>11:39:02</v>
       </c>
       <c r="E54" t="str">
         <v>Manual</v>
@@ -1484,7 +1484,7 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>190314</v>
+        <v>202162</v>
       </c>
       <c r="B55" t="str">
         <v>General Surgery</v>
@@ -1493,7 +1493,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D55" t="str">
-        <v>11:39:02</v>
+        <v>11:39:12</v>
       </c>
       <c r="E55" t="str">
         <v>Manual</v>
@@ -1504,7 +1504,7 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>202162</v>
+        <v>201819</v>
       </c>
       <c r="B56" t="str">
         <v>General Surgery</v>
@@ -1513,7 +1513,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D56" t="str">
-        <v>11:39:12</v>
+        <v>11:39:21</v>
       </c>
       <c r="E56" t="str">
         <v>Manual</v>
@@ -1524,7 +1524,7 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>201819</v>
+        <v>201990</v>
       </c>
       <c r="B57" t="str">
         <v>General Surgery</v>
@@ -1533,7 +1533,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D57" t="str">
-        <v>11:39:21</v>
+        <v>11:39:29</v>
       </c>
       <c r="E57" t="str">
         <v>Manual</v>
@@ -1544,7 +1544,7 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>201990</v>
+        <v>211175</v>
       </c>
       <c r="B58" t="str">
         <v>General Surgery</v>
@@ -1553,7 +1553,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D58" t="str">
-        <v>11:39:29</v>
+        <v>11:39:42</v>
       </c>
       <c r="E58" t="str">
         <v>Manual</v>
@@ -1564,7 +1564,7 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>211175</v>
+        <v>201795</v>
       </c>
       <c r="B59" t="str">
         <v>General Surgery</v>
@@ -1573,7 +1573,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D59" t="str">
-        <v>11:39:42</v>
+        <v>11:39:58</v>
       </c>
       <c r="E59" t="str">
         <v>Manual</v>
@@ -1584,7 +1584,7 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>201795</v>
+        <v>211174</v>
       </c>
       <c r="B60" t="str">
         <v>General Surgery</v>
@@ -1593,7 +1593,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D60" t="str">
-        <v>11:39:58</v>
+        <v>11:41:21</v>
       </c>
       <c r="E60" t="str">
         <v>Manual</v>
@@ -1604,7 +1604,7 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>211174</v>
+        <v>211092</v>
       </c>
       <c r="B61" t="str">
         <v>General Surgery</v>
@@ -1613,7 +1613,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D61" t="str">
-        <v>11:41:21</v>
+        <v>11:41:29</v>
       </c>
       <c r="E61" t="str">
         <v>Manual</v>
@@ -1624,7 +1624,7 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>211092</v>
+        <v>211046</v>
       </c>
       <c r="B62" t="str">
         <v>General Surgery</v>
@@ -1633,7 +1633,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D62" t="str">
-        <v>11:41:29</v>
+        <v>11:41:38</v>
       </c>
       <c r="E62" t="str">
         <v>Manual</v>
@@ -1644,7 +1644,7 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>211046</v>
+        <v>211242</v>
       </c>
       <c r="B63" t="str">
         <v>General Surgery</v>
@@ -1653,7 +1653,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D63" t="str">
-        <v>11:41:38</v>
+        <v>11:41:50</v>
       </c>
       <c r="E63" t="str">
         <v>Manual</v>
@@ -1664,7 +1664,7 @@
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>211242</v>
+        <v>211010</v>
       </c>
       <c r="B64" t="str">
         <v>General Surgery</v>
@@ -1673,7 +1673,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D64" t="str">
-        <v>11:41:50</v>
+        <v>11:41:58</v>
       </c>
       <c r="E64" t="str">
         <v>Manual</v>
@@ -1684,7 +1684,7 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>211010</v>
+        <v>190968</v>
       </c>
       <c r="B65" t="str">
         <v>General Surgery</v>
@@ -1693,7 +1693,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D65" t="str">
-        <v>11:41:58</v>
+        <v>11:42:09</v>
       </c>
       <c r="E65" t="str">
         <v>Manual</v>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>190968</v>
+        <v>200933</v>
       </c>
       <c r="B66" t="str">
         <v>General Surgery</v>
@@ -1713,7 +1713,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D66" t="str">
-        <v>11:42:09</v>
+        <v>11:42:20</v>
       </c>
       <c r="E66" t="str">
         <v>Manual</v>
@@ -1724,7 +1724,7 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>200933</v>
+        <v>201825</v>
       </c>
       <c r="B67" t="str">
         <v>General Surgery</v>
@@ -1733,7 +1733,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D67" t="str">
-        <v>11:42:20</v>
+        <v>11:42:35</v>
       </c>
       <c r="E67" t="str">
         <v>Manual</v>
@@ -1744,7 +1744,7 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>201825</v>
+        <v>190801</v>
       </c>
       <c r="B68" t="str">
         <v>General Surgery</v>
@@ -1753,7 +1753,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D68" t="str">
-        <v>11:42:35</v>
+        <v>11:42:42</v>
       </c>
       <c r="E68" t="str">
         <v>Manual</v>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>190801</v>
+        <v>201465</v>
       </c>
       <c r="B69" t="str">
         <v>General Surgery</v>
@@ -1773,10 +1773,10 @@
         <v>11/10/2025</v>
       </c>
       <c r="D69" t="str">
-        <v>11:42:42</v>
+        <v>11:42:49</v>
       </c>
       <c r="E69" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F69" t="str">
         <v>dnasr281@gmail.com</v>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>201465</v>
+        <v>201171</v>
       </c>
       <c r="B70" t="str">
         <v>General Surgery</v>
@@ -1793,7 +1793,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D70" t="str">
-        <v>11:42:49</v>
+        <v>11:42:52</v>
       </c>
       <c r="E70" t="str">
         <v>Scan</v>
@@ -1804,7 +1804,7 @@
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>201171</v>
+        <v>200491</v>
       </c>
       <c r="B71" t="str">
         <v>General Surgery</v>
@@ -1813,7 +1813,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D71" t="str">
-        <v>11:42:52</v>
+        <v>11:42:54</v>
       </c>
       <c r="E71" t="str">
         <v>Scan</v>
@@ -1824,7 +1824,7 @@
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>200491</v>
+        <v>200490</v>
       </c>
       <c r="B72" t="str">
         <v>General Surgery</v>
@@ -1833,7 +1833,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D72" t="str">
-        <v>11:42:54</v>
+        <v>11:42:56</v>
       </c>
       <c r="E72" t="str">
         <v>Scan</v>
@@ -1844,7 +1844,7 @@
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>200490</v>
+        <v>200228</v>
       </c>
       <c r="B73" t="str">
         <v>General Surgery</v>
@@ -1853,7 +1853,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D73" t="str">
-        <v>11:42:56</v>
+        <v>11:42:59</v>
       </c>
       <c r="E73" t="str">
         <v>Scan</v>
@@ -1864,7 +1864,7 @@
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>200228</v>
+        <v>201669</v>
       </c>
       <c r="B74" t="str">
         <v>General Surgery</v>
@@ -1873,7 +1873,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D74" t="str">
-        <v>11:42:59</v>
+        <v>11:43:01</v>
       </c>
       <c r="E74" t="str">
         <v>Scan</v>
@@ -1884,7 +1884,7 @@
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>201669</v>
+        <v>202004</v>
       </c>
       <c r="B75" t="str">
         <v>General Surgery</v>
@@ -1893,7 +1893,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D75" t="str">
-        <v>11:43:01</v>
+        <v>11:43:03</v>
       </c>
       <c r="E75" t="str">
         <v>Scan</v>
@@ -1904,7 +1904,7 @@
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>202004</v>
+        <v>200116</v>
       </c>
       <c r="B76" t="str">
         <v>General Surgery</v>
@@ -1913,7 +1913,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D76" t="str">
-        <v>11:43:03</v>
+        <v>11:43:05</v>
       </c>
       <c r="E76" t="str">
         <v>Scan</v>
@@ -1924,7 +1924,7 @@
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>200116</v>
+        <v>190796</v>
       </c>
       <c r="B77" t="str">
         <v>General Surgery</v>
@@ -1933,7 +1933,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D77" t="str">
-        <v>11:43:05</v>
+        <v>11:43:07</v>
       </c>
       <c r="E77" t="str">
         <v>Scan</v>
@@ -1944,7 +1944,7 @@
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>190796</v>
+        <v>190981</v>
       </c>
       <c r="B78" t="str">
         <v>General Surgery</v>
@@ -1953,7 +1953,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D78" t="str">
-        <v>11:43:07</v>
+        <v>11:43:09</v>
       </c>
       <c r="E78" t="str">
         <v>Scan</v>
@@ -1964,7 +1964,7 @@
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>190981</v>
+        <v>200163</v>
       </c>
       <c r="B79" t="str">
         <v>General Surgery</v>
@@ -1973,7 +1973,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D79" t="str">
-        <v>11:43:09</v>
+        <v>11:43:12</v>
       </c>
       <c r="E79" t="str">
         <v>Scan</v>
@@ -1984,7 +1984,7 @@
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>200163</v>
+        <v>191061</v>
       </c>
       <c r="B80" t="str">
         <v>General Surgery</v>
@@ -1993,7 +1993,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D80" t="str">
-        <v>11:43:12</v>
+        <v>11:43:15</v>
       </c>
       <c r="E80" t="str">
         <v>Scan</v>
@@ -2004,7 +2004,7 @@
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>191061</v>
+        <v>200744</v>
       </c>
       <c r="B81" t="str">
         <v>General Surgery</v>
@@ -2013,7 +2013,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D81" t="str">
-        <v>11:43:15</v>
+        <v>11:43:17</v>
       </c>
       <c r="E81" t="str">
         <v>Scan</v>
@@ -2024,7 +2024,7 @@
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>200744</v>
+        <v>201564</v>
       </c>
       <c r="B82" t="str">
         <v>General Surgery</v>
@@ -2033,7 +2033,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D82" t="str">
-        <v>11:43:17</v>
+        <v>11:43:20</v>
       </c>
       <c r="E82" t="str">
         <v>Scan</v>
@@ -2044,7 +2044,7 @@
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>201564</v>
+        <v>200804</v>
       </c>
       <c r="B83" t="str">
         <v>General Surgery</v>
@@ -2053,7 +2053,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D83" t="str">
-        <v>11:43:20</v>
+        <v>11:43:22</v>
       </c>
       <c r="E83" t="str">
         <v>Scan</v>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>200804</v>
+        <v>200792</v>
       </c>
       <c r="B84" t="str">
         <v>General Surgery</v>
@@ -2073,7 +2073,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D84" t="str">
-        <v>11:43:22</v>
+        <v>11:43:24</v>
       </c>
       <c r="E84" t="str">
         <v>Scan</v>
@@ -2084,7 +2084,7 @@
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>200792</v>
+        <v>200628</v>
       </c>
       <c r="B85" t="str">
         <v>General Surgery</v>
@@ -2093,7 +2093,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D85" t="str">
-        <v>11:43:24</v>
+        <v>11:43:26</v>
       </c>
       <c r="E85" t="str">
         <v>Scan</v>
@@ -2104,7 +2104,7 @@
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>200628</v>
+        <v>211216</v>
       </c>
       <c r="B86" t="str">
         <v>General Surgery</v>
@@ -2113,7 +2113,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D86" t="str">
-        <v>11:43:26</v>
+        <v>11:43:28</v>
       </c>
       <c r="E86" t="str">
         <v>Scan</v>
@@ -2124,7 +2124,7 @@
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>211216</v>
+        <v>211197</v>
       </c>
       <c r="B87" t="str">
         <v>General Surgery</v>
@@ -2133,7 +2133,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D87" t="str">
-        <v>11:43:28</v>
+        <v>11:43:31</v>
       </c>
       <c r="E87" t="str">
         <v>Scan</v>
@@ -2144,7 +2144,7 @@
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>211197</v>
+        <v>201397</v>
       </c>
       <c r="B88" t="str">
         <v>General Surgery</v>
@@ -2153,7 +2153,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D88" t="str">
-        <v>11:43:31</v>
+        <v>11:43:33</v>
       </c>
       <c r="E88" t="str">
         <v>Scan</v>
@@ -2164,7 +2164,7 @@
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>201397</v>
+        <v>200917</v>
       </c>
       <c r="B89" t="str">
         <v>General Surgery</v>
@@ -2173,7 +2173,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D89" t="str">
-        <v>11:43:33</v>
+        <v>11:43:35</v>
       </c>
       <c r="E89" t="str">
         <v>Scan</v>
@@ -2184,7 +2184,7 @@
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>200917</v>
+        <v>201051</v>
       </c>
       <c r="B90" t="str">
         <v>General Surgery</v>
@@ -2193,7 +2193,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D90" t="str">
-        <v>11:43:35</v>
+        <v>11:43:37</v>
       </c>
       <c r="E90" t="str">
         <v>Scan</v>
@@ -2204,7 +2204,7 @@
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>201051</v>
+        <v>201501</v>
       </c>
       <c r="B91" t="str">
         <v>General Surgery</v>
@@ -2213,7 +2213,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D91" t="str">
-        <v>11:43:37</v>
+        <v>11:43:40</v>
       </c>
       <c r="E91" t="str">
         <v>Scan</v>
@@ -2224,7 +2224,7 @@
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>201501</v>
+        <v>200905</v>
       </c>
       <c r="B92" t="str">
         <v>General Surgery</v>
@@ -2233,7 +2233,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D92" t="str">
-        <v>11:43:40</v>
+        <v>11:43:42</v>
       </c>
       <c r="E92" t="str">
         <v>Scan</v>
@@ -2244,7 +2244,7 @@
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>200905</v>
+        <v>200938</v>
       </c>
       <c r="B93" t="str">
         <v>General Surgery</v>
@@ -2253,7 +2253,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D93" t="str">
-        <v>11:43:42</v>
+        <v>11:43:45</v>
       </c>
       <c r="E93" t="str">
         <v>Scan</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>200938</v>
+        <v>211043</v>
       </c>
       <c r="B94" t="str">
         <v>General Surgery</v>
@@ -2273,7 +2273,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D94" t="str">
-        <v>11:43:45</v>
+        <v>11:43:47</v>
       </c>
       <c r="E94" t="str">
         <v>Scan</v>
@@ -2284,7 +2284,7 @@
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>211043</v>
+        <v>211133</v>
       </c>
       <c r="B95" t="str">
         <v>General Surgery</v>
@@ -2293,7 +2293,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D95" t="str">
-        <v>11:43:47</v>
+        <v>11:43:49</v>
       </c>
       <c r="E95" t="str">
         <v>Scan</v>
@@ -2304,7 +2304,7 @@
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>211133</v>
+        <v>211741</v>
       </c>
       <c r="B96" t="str">
         <v>General Surgery</v>
@@ -2313,7 +2313,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D96" t="str">
-        <v>11:43:49</v>
+        <v>11:43:50</v>
       </c>
       <c r="E96" t="str">
         <v>Scan</v>
@@ -2324,7 +2324,7 @@
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>211741</v>
+        <v>211245</v>
       </c>
       <c r="B97" t="str">
         <v>General Surgery</v>
@@ -2333,7 +2333,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D97" t="str">
-        <v>11:43:50</v>
+        <v>11:43:52</v>
       </c>
       <c r="E97" t="str">
         <v>Scan</v>
@@ -2344,7 +2344,7 @@
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>211245</v>
+        <v>190929</v>
       </c>
       <c r="B98" t="str">
         <v>General Surgery</v>
@@ -2353,7 +2353,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D98" t="str">
-        <v>11:43:52</v>
+        <v>11:43:55</v>
       </c>
       <c r="E98" t="str">
         <v>Scan</v>
@@ -2364,7 +2364,7 @@
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>190929</v>
+        <v>191119</v>
       </c>
       <c r="B99" t="str">
         <v>General Surgery</v>
@@ -2373,7 +2373,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D99" t="str">
-        <v>11:43:55</v>
+        <v>11:43:56</v>
       </c>
       <c r="E99" t="str">
         <v>Scan</v>
@@ -2384,7 +2384,7 @@
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>191119</v>
+        <v>211210</v>
       </c>
       <c r="B100" t="str">
         <v>General Surgery</v>
@@ -2393,10 +2393,10 @@
         <v>11/10/2025</v>
       </c>
       <c r="D100" t="str">
-        <v>11:43:56</v>
+        <v>11:44:43</v>
       </c>
       <c r="E100" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F100" t="str">
         <v>dnasr281@gmail.com</v>
@@ -2404,7 +2404,7 @@
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>211210</v>
+        <v>201880</v>
       </c>
       <c r="B101" t="str">
         <v>General Surgery</v>
@@ -2413,7 +2413,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D101" t="str">
-        <v>11:44:43</v>
+        <v>11:45:28</v>
       </c>
       <c r="E101" t="str">
         <v>Manual</v>
@@ -2424,7 +2424,7 @@
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>201880</v>
+        <v>211246</v>
       </c>
       <c r="B102" t="str">
         <v>General Surgery</v>
@@ -2433,7 +2433,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D102" t="str">
-        <v>11:45:28</v>
+        <v>11:45:59</v>
       </c>
       <c r="E102" t="str">
         <v>Manual</v>
@@ -2444,7 +2444,7 @@
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>211246</v>
+        <v>201823</v>
       </c>
       <c r="B103" t="str">
         <v>General Surgery</v>
@@ -2453,7 +2453,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D103" t="str">
-        <v>11:45:59</v>
+        <v>11:46:33</v>
       </c>
       <c r="E103" t="str">
         <v>Manual</v>
@@ -2464,7 +2464,7 @@
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>201823</v>
+        <v>200928</v>
       </c>
       <c r="B104" t="str">
         <v>General Surgery</v>
@@ -2473,7 +2473,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D104" t="str">
-        <v>11:46:33</v>
+        <v>11:47:11</v>
       </c>
       <c r="E104" t="str">
         <v>Manual</v>
@@ -2484,7 +2484,7 @@
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>200928</v>
+        <v>201237</v>
       </c>
       <c r="B105" t="str">
         <v>General Surgery</v>
@@ -2493,7 +2493,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D105" t="str">
-        <v>11:47:11</v>
+        <v>11:47:35</v>
       </c>
       <c r="E105" t="str">
         <v>Manual</v>
@@ -2504,7 +2504,7 @@
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>201237</v>
+        <v>201513</v>
       </c>
       <c r="B106" t="str">
         <v>General Surgery</v>
@@ -2513,7 +2513,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D106" t="str">
-        <v>11:47:35</v>
+        <v>11:48:02</v>
       </c>
       <c r="E106" t="str">
         <v>Manual</v>
@@ -2524,7 +2524,7 @@
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>201513</v>
+        <v>200997</v>
       </c>
       <c r="B107" t="str">
         <v>General Surgery</v>
@@ -2533,7 +2533,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D107" t="str">
-        <v>11:48:02</v>
+        <v>11:48:26</v>
       </c>
       <c r="E107" t="str">
         <v>Manual</v>
@@ -2544,7 +2544,7 @@
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>200997</v>
+        <v>181004</v>
       </c>
       <c r="B108" t="str">
         <v>General Surgery</v>
@@ -2553,7 +2553,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D108" t="str">
-        <v>11:48:26</v>
+        <v>11:48:49</v>
       </c>
       <c r="E108" t="str">
         <v>Manual</v>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>181004</v>
+        <v>211121</v>
       </c>
       <c r="B109" t="str">
         <v>General Surgery</v>
@@ -2573,7 +2573,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D109" t="str">
-        <v>11:48:49</v>
+        <v>11:49:14</v>
       </c>
       <c r="E109" t="str">
         <v>Manual</v>
@@ -2584,7 +2584,7 @@
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>211121</v>
+        <v>201252</v>
       </c>
       <c r="B110" t="str">
         <v>General Surgery</v>
@@ -2593,7 +2593,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D110" t="str">
-        <v>11:49:14</v>
+        <v>11:49:29</v>
       </c>
       <c r="E110" t="str">
         <v>Manual</v>
@@ -2604,7 +2604,7 @@
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>201252</v>
+        <v>201023</v>
       </c>
       <c r="B111" t="str">
         <v>General Surgery</v>
@@ -2613,7 +2613,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D111" t="str">
-        <v>11:49:29</v>
+        <v>11:49:42</v>
       </c>
       <c r="E111" t="str">
         <v>Manual</v>
@@ -2624,7 +2624,7 @@
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>201023</v>
+        <v>201253</v>
       </c>
       <c r="B112" t="str">
         <v>General Surgery</v>
@@ -2633,7 +2633,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D112" t="str">
-        <v>11:49:42</v>
+        <v>11:49:57</v>
       </c>
       <c r="E112" t="str">
         <v>Manual</v>
@@ -2644,7 +2644,7 @@
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>201253</v>
+        <v>201337</v>
       </c>
       <c r="B113" t="str">
         <v>General Surgery</v>
@@ -2653,7 +2653,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D113" t="str">
-        <v>11:49:57</v>
+        <v>11:50:11</v>
       </c>
       <c r="E113" t="str">
         <v>Manual</v>
@@ -2664,7 +2664,7 @@
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>201337</v>
+        <v>201572</v>
       </c>
       <c r="B114" t="str">
         <v>General Surgery</v>
@@ -2673,10 +2673,10 @@
         <v>11/10/2025</v>
       </c>
       <c r="D114" t="str">
-        <v>11:50:11</v>
+        <v>11:50:20</v>
       </c>
       <c r="E114" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F114" t="str">
         <v>dnasr281@gmail.com</v>
@@ -2684,7 +2684,7 @@
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>201572</v>
+        <v>201398</v>
       </c>
       <c r="B115" t="str">
         <v>General Surgery</v>
@@ -2693,38 +2693,18 @@
         <v>11/10/2025</v>
       </c>
       <c r="D115" t="str">
-        <v>11:50:20</v>
+        <v>11:50:41</v>
       </c>
       <c r="E115" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F115" t="str">
-        <v>dnasr281@gmail.com</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="str">
-        <v>201398</v>
-      </c>
-      <c r="B116" t="str">
-        <v>General Surgery</v>
-      </c>
-      <c r="C116" t="str">
-        <v>11/10/2025</v>
-      </c>
-      <c r="D116" t="str">
-        <v>11:50:41</v>
-      </c>
-      <c r="E116" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F116" t="str">
         <v>dnasr281@gmail.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F116"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F115"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update edited session - 2025-10-11T10:07:06.345Z - Cache Bust ID: 1760177226345o3f2no22s
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_General_Surgery_scanner1760170816881_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
+++ b/log_history/Y4_B2526_General_Surgery_scanner1760170816881_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="General_Surgery" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F115"/>
+  <dimension ref="A1:F114"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -624,7 +624,7 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>200852</v>
+        <v>200003</v>
       </c>
       <c r="B12" t="str">
         <v>General Surgery</v>
@@ -633,7 +633,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D12" t="str">
-        <v>11:23:31</v>
+        <v>11:23:43</v>
       </c>
       <c r="E12" t="str">
         <v>Manual</v>
@@ -644,7 +644,7 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>200003</v>
+        <v>201682</v>
       </c>
       <c r="B13" t="str">
         <v>General Surgery</v>
@@ -653,7 +653,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D13" t="str">
-        <v>11:23:43</v>
+        <v>11:24:03</v>
       </c>
       <c r="E13" t="str">
         <v>Manual</v>
@@ -664,7 +664,7 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>201682</v>
+        <v>200405</v>
       </c>
       <c r="B14" t="str">
         <v>General Surgery</v>
@@ -673,7 +673,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D14" t="str">
-        <v>11:24:03</v>
+        <v>11:24:11</v>
       </c>
       <c r="E14" t="str">
         <v>Manual</v>
@@ -684,7 +684,7 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>200405</v>
+        <v>200877</v>
       </c>
       <c r="B15" t="str">
         <v>General Surgery</v>
@@ -693,7 +693,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D15" t="str">
-        <v>11:24:11</v>
+        <v>11:24:44</v>
       </c>
       <c r="E15" t="str">
         <v>Manual</v>
@@ -704,7 +704,7 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>200877</v>
+        <v>191480</v>
       </c>
       <c r="B16" t="str">
         <v>General Surgery</v>
@@ -713,7 +713,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D16" t="str">
-        <v>11:24:44</v>
+        <v>11:24:53</v>
       </c>
       <c r="E16" t="str">
         <v>Manual</v>
@@ -724,7 +724,7 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>191480</v>
+        <v>191375</v>
       </c>
       <c r="B17" t="str">
         <v>General Surgery</v>
@@ -733,7 +733,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D17" t="str">
-        <v>11:24:53</v>
+        <v>11:25:26</v>
       </c>
       <c r="E17" t="str">
         <v>Manual</v>
@@ -744,7 +744,7 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>191375</v>
+        <v>201218</v>
       </c>
       <c r="B18" t="str">
         <v>General Surgery</v>
@@ -753,7 +753,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D18" t="str">
-        <v>11:25:26</v>
+        <v>11:25:32</v>
       </c>
       <c r="E18" t="str">
         <v>Manual</v>
@@ -764,7 +764,7 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>201218</v>
+        <v>201438</v>
       </c>
       <c r="B19" t="str">
         <v>General Surgery</v>
@@ -773,7 +773,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D19" t="str">
-        <v>11:25:32</v>
+        <v>11:25:50</v>
       </c>
       <c r="E19" t="str">
         <v>Manual</v>
@@ -784,7 +784,7 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>201438</v>
+        <v>191186</v>
       </c>
       <c r="B20" t="str">
         <v>General Surgery</v>
@@ -793,7 +793,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D20" t="str">
-        <v>11:25:50</v>
+        <v>11:26:11</v>
       </c>
       <c r="E20" t="str">
         <v>Manual</v>
@@ -804,7 +804,7 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>191186</v>
+        <v>191258</v>
       </c>
       <c r="B21" t="str">
         <v>General Surgery</v>
@@ -813,7 +813,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D21" t="str">
-        <v>11:26:11</v>
+        <v>11:27:36</v>
       </c>
       <c r="E21" t="str">
         <v>Manual</v>
@@ -824,7 +824,7 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>191258</v>
+        <v>200742</v>
       </c>
       <c r="B22" t="str">
         <v>General Surgery</v>
@@ -833,7 +833,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D22" t="str">
-        <v>11:27:36</v>
+        <v>11:27:56</v>
       </c>
       <c r="E22" t="str">
         <v>Manual</v>
@@ -844,7 +844,7 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>200742</v>
+        <v>201563</v>
       </c>
       <c r="B23" t="str">
         <v>General Surgery</v>
@@ -853,7 +853,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D23" t="str">
-        <v>11:27:56</v>
+        <v>11:28:13</v>
       </c>
       <c r="E23" t="str">
         <v>Manual</v>
@@ -864,7 +864,7 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>201563</v>
+        <v>180804</v>
       </c>
       <c r="B24" t="str">
         <v>General Surgery</v>
@@ -873,7 +873,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D24" t="str">
-        <v>11:28:13</v>
+        <v>11:28:23</v>
       </c>
       <c r="E24" t="str">
         <v>Manual</v>
@@ -884,7 +884,7 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>180804</v>
+        <v>211167</v>
       </c>
       <c r="B25" t="str">
         <v>General Surgery</v>
@@ -893,7 +893,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D25" t="str">
-        <v>11:28:23</v>
+        <v>11:28:31</v>
       </c>
       <c r="E25" t="str">
         <v>Manual</v>
@@ -904,7 +904,7 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>211167</v>
+        <v>211169</v>
       </c>
       <c r="B26" t="str">
         <v>General Surgery</v>
@@ -913,7 +913,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D26" t="str">
-        <v>11:28:31</v>
+        <v>11:28:41</v>
       </c>
       <c r="E26" t="str">
         <v>Manual</v>
@@ -924,7 +924,7 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>211169</v>
+        <v>211079</v>
       </c>
       <c r="B27" t="str">
         <v>General Surgery</v>
@@ -933,7 +933,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D27" t="str">
-        <v>11:28:41</v>
+        <v>11:28:48</v>
       </c>
       <c r="E27" t="str">
         <v>Manual</v>
@@ -944,7 +944,7 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>211079</v>
+        <v>200468</v>
       </c>
       <c r="B28" t="str">
         <v>General Surgery</v>
@@ -953,7 +953,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D28" t="str">
-        <v>11:28:48</v>
+        <v>11:29:01</v>
       </c>
       <c r="E28" t="str">
         <v>Manual</v>
@@ -964,7 +964,7 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>200468</v>
+        <v>191109</v>
       </c>
       <c r="B29" t="str">
         <v>General Surgery</v>
@@ -973,7 +973,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D29" t="str">
-        <v>11:29:01</v>
+        <v>11:29:08</v>
       </c>
       <c r="E29" t="str">
         <v>Manual</v>
@@ -984,7 +984,7 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>191109</v>
+        <v>191088</v>
       </c>
       <c r="B30" t="str">
         <v>General Surgery</v>
@@ -993,7 +993,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D30" t="str">
-        <v>11:29:08</v>
+        <v>11:29:17</v>
       </c>
       <c r="E30" t="str">
         <v>Manual</v>
@@ -1004,7 +1004,7 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>191088</v>
+        <v>200423</v>
       </c>
       <c r="B31" t="str">
         <v>General Surgery</v>
@@ -1013,7 +1013,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D31" t="str">
-        <v>11:29:17</v>
+        <v>11:29:25</v>
       </c>
       <c r="E31" t="str">
         <v>Manual</v>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>200423</v>
+        <v>190931</v>
       </c>
       <c r="B32" t="str">
         <v>General Surgery</v>
@@ -1033,7 +1033,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D32" t="str">
-        <v>11:29:25</v>
+        <v>11:29:35</v>
       </c>
       <c r="E32" t="str">
         <v>Manual</v>
@@ -1044,7 +1044,7 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>190931</v>
+        <v>190922</v>
       </c>
       <c r="B33" t="str">
         <v>General Surgery</v>
@@ -1053,7 +1053,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D33" t="str">
-        <v>11:29:35</v>
+        <v>11:29:50</v>
       </c>
       <c r="E33" t="str">
         <v>Manual</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>190922</v>
+        <v>191131</v>
       </c>
       <c r="B34" t="str">
         <v>General Surgery</v>
@@ -1073,7 +1073,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D34" t="str">
-        <v>11:29:50</v>
+        <v>11:30:02</v>
       </c>
       <c r="E34" t="str">
         <v>Manual</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>191131</v>
+        <v>190803</v>
       </c>
       <c r="B35" t="str">
         <v>General Surgery</v>
@@ -1093,7 +1093,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D35" t="str">
-        <v>11:30:02</v>
+        <v>11:30:15</v>
       </c>
       <c r="E35" t="str">
         <v>Manual</v>
@@ -1104,7 +1104,7 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>190803</v>
+        <v>181013</v>
       </c>
       <c r="B36" t="str">
         <v>General Surgery</v>
@@ -1113,7 +1113,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D36" t="str">
-        <v>11:30:15</v>
+        <v>11:30:22</v>
       </c>
       <c r="E36" t="str">
         <v>Manual</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>181013</v>
+        <v>201495</v>
       </c>
       <c r="B37" t="str">
         <v>General Surgery</v>
@@ -1133,7 +1133,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D37" t="str">
-        <v>11:30:22</v>
+        <v>11:30:50</v>
       </c>
       <c r="E37" t="str">
         <v>Manual</v>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>201495</v>
+        <v>201026</v>
       </c>
       <c r="B38" t="str">
         <v>General Surgery</v>
@@ -1153,7 +1153,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D38" t="str">
-        <v>11:30:50</v>
+        <v>11:33:15</v>
       </c>
       <c r="E38" t="str">
         <v>Manual</v>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>201026</v>
+        <v>200850</v>
       </c>
       <c r="B39" t="str">
         <v>General Surgery</v>
@@ -1173,7 +1173,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D39" t="str">
-        <v>11:33:15</v>
+        <v>11:33:26</v>
       </c>
       <c r="E39" t="str">
         <v>Manual</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>200850</v>
+        <v>200866</v>
       </c>
       <c r="B40" t="str">
         <v>General Surgery</v>
@@ -1193,7 +1193,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D40" t="str">
-        <v>11:33:26</v>
+        <v>11:33:36</v>
       </c>
       <c r="E40" t="str">
         <v>Manual</v>
@@ -1204,7 +1204,7 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>200866</v>
+        <v>201834</v>
       </c>
       <c r="B41" t="str">
         <v>General Surgery</v>
@@ -1213,7 +1213,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D41" t="str">
-        <v>11:33:36</v>
+        <v>11:35:22</v>
       </c>
       <c r="E41" t="str">
         <v>Manual</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>201834</v>
+        <v>211118</v>
       </c>
       <c r="B42" t="str">
         <v>General Surgery</v>
@@ -1233,7 +1233,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D42" t="str">
-        <v>11:35:22</v>
+        <v>11:36:25</v>
       </c>
       <c r="E42" t="str">
         <v>Manual</v>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>211118</v>
+        <v>200904</v>
       </c>
       <c r="B43" t="str">
         <v>General Surgery</v>
@@ -1253,7 +1253,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D43" t="str">
-        <v>11:36:25</v>
+        <v>11:37:01</v>
       </c>
       <c r="E43" t="str">
         <v>Manual</v>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>200904</v>
+        <v>201632</v>
       </c>
       <c r="B44" t="str">
         <v>General Surgery</v>
@@ -1273,7 +1273,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D44" t="str">
-        <v>11:37:01</v>
+        <v>11:37:08</v>
       </c>
       <c r="E44" t="str">
         <v>Manual</v>
@@ -1284,7 +1284,7 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>201632</v>
+        <v>201190</v>
       </c>
       <c r="B45" t="str">
         <v>General Surgery</v>
@@ -1293,7 +1293,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D45" t="str">
-        <v>11:37:08</v>
+        <v>11:37:15</v>
       </c>
       <c r="E45" t="str">
         <v>Manual</v>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>201190</v>
+        <v>200824</v>
       </c>
       <c r="B46" t="str">
         <v>General Surgery</v>
@@ -1313,7 +1313,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D46" t="str">
-        <v>11:37:15</v>
+        <v>11:37:21</v>
       </c>
       <c r="E46" t="str">
         <v>Manual</v>
@@ -1324,7 +1324,7 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>200824</v>
+        <v>201197</v>
       </c>
       <c r="B47" t="str">
         <v>General Surgery</v>
@@ -1333,7 +1333,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D47" t="str">
-        <v>11:37:21</v>
+        <v>11:37:28</v>
       </c>
       <c r="E47" t="str">
         <v>Manual</v>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>201197</v>
+        <v>200914</v>
       </c>
       <c r="B48" t="str">
         <v>General Surgery</v>
@@ -1353,7 +1353,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D48" t="str">
-        <v>11:37:28</v>
+        <v>11:37:39</v>
       </c>
       <c r="E48" t="str">
         <v>Manual</v>
@@ -1364,7 +1364,7 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>200914</v>
+        <v>201065</v>
       </c>
       <c r="B49" t="str">
         <v>General Surgery</v>
@@ -1373,7 +1373,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D49" t="str">
-        <v>11:37:39</v>
+        <v>11:38:11</v>
       </c>
       <c r="E49" t="str">
         <v>Manual</v>
@@ -1384,7 +1384,7 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>201065</v>
+        <v>191478</v>
       </c>
       <c r="B50" t="str">
         <v>General Surgery</v>
@@ -1393,7 +1393,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D50" t="str">
-        <v>11:38:11</v>
+        <v>11:38:32</v>
       </c>
       <c r="E50" t="str">
         <v>Manual</v>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>191478</v>
+        <v>200999</v>
       </c>
       <c r="B51" t="str">
         <v>General Surgery</v>
@@ -1413,7 +1413,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D51" t="str">
-        <v>11:38:32</v>
+        <v>11:38:40</v>
       </c>
       <c r="E51" t="str">
         <v>Manual</v>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>200999</v>
+        <v>201157</v>
       </c>
       <c r="B52" t="str">
         <v>General Surgery</v>
@@ -1433,7 +1433,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D52" t="str">
-        <v>11:38:40</v>
+        <v>11:38:51</v>
       </c>
       <c r="E52" t="str">
         <v>Manual</v>
@@ -1444,7 +1444,7 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>201157</v>
+        <v>190314</v>
       </c>
       <c r="B53" t="str">
         <v>General Surgery</v>
@@ -1453,7 +1453,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D53" t="str">
-        <v>11:38:51</v>
+        <v>11:39:02</v>
       </c>
       <c r="E53" t="str">
         <v>Manual</v>
@@ -1464,7 +1464,7 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>190314</v>
+        <v>202162</v>
       </c>
       <c r="B54" t="str">
         <v>General Surgery</v>
@@ -1473,7 +1473,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D54" t="str">
-        <v>11:39:02</v>
+        <v>11:39:12</v>
       </c>
       <c r="E54" t="str">
         <v>Manual</v>
@@ -1484,7 +1484,7 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>202162</v>
+        <v>201819</v>
       </c>
       <c r="B55" t="str">
         <v>General Surgery</v>
@@ -1493,7 +1493,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D55" t="str">
-        <v>11:39:12</v>
+        <v>11:39:21</v>
       </c>
       <c r="E55" t="str">
         <v>Manual</v>
@@ -1504,7 +1504,7 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>201819</v>
+        <v>201990</v>
       </c>
       <c r="B56" t="str">
         <v>General Surgery</v>
@@ -1513,7 +1513,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D56" t="str">
-        <v>11:39:21</v>
+        <v>11:39:29</v>
       </c>
       <c r="E56" t="str">
         <v>Manual</v>
@@ -1524,7 +1524,7 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>201990</v>
+        <v>211175</v>
       </c>
       <c r="B57" t="str">
         <v>General Surgery</v>
@@ -1533,7 +1533,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D57" t="str">
-        <v>11:39:29</v>
+        <v>11:39:42</v>
       </c>
       <c r="E57" t="str">
         <v>Manual</v>
@@ -1544,7 +1544,7 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>211175</v>
+        <v>201795</v>
       </c>
       <c r="B58" t="str">
         <v>General Surgery</v>
@@ -1553,7 +1553,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D58" t="str">
-        <v>11:39:42</v>
+        <v>11:39:58</v>
       </c>
       <c r="E58" t="str">
         <v>Manual</v>
@@ -1564,7 +1564,7 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>201795</v>
+        <v>211174</v>
       </c>
       <c r="B59" t="str">
         <v>General Surgery</v>
@@ -1573,7 +1573,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D59" t="str">
-        <v>11:39:58</v>
+        <v>11:41:21</v>
       </c>
       <c r="E59" t="str">
         <v>Manual</v>
@@ -1584,7 +1584,7 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>211174</v>
+        <v>211092</v>
       </c>
       <c r="B60" t="str">
         <v>General Surgery</v>
@@ -1593,7 +1593,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D60" t="str">
-        <v>11:41:21</v>
+        <v>11:41:29</v>
       </c>
       <c r="E60" t="str">
         <v>Manual</v>
@@ -1604,7 +1604,7 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>211092</v>
+        <v>211046</v>
       </c>
       <c r="B61" t="str">
         <v>General Surgery</v>
@@ -1613,7 +1613,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D61" t="str">
-        <v>11:41:29</v>
+        <v>11:41:38</v>
       </c>
       <c r="E61" t="str">
         <v>Manual</v>
@@ -1624,7 +1624,7 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>211046</v>
+        <v>211242</v>
       </c>
       <c r="B62" t="str">
         <v>General Surgery</v>
@@ -1633,7 +1633,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D62" t="str">
-        <v>11:41:38</v>
+        <v>11:41:50</v>
       </c>
       <c r="E62" t="str">
         <v>Manual</v>
@@ -1644,7 +1644,7 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>211242</v>
+        <v>211010</v>
       </c>
       <c r="B63" t="str">
         <v>General Surgery</v>
@@ -1653,7 +1653,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D63" t="str">
-        <v>11:41:50</v>
+        <v>11:41:58</v>
       </c>
       <c r="E63" t="str">
         <v>Manual</v>
@@ -1664,7 +1664,7 @@
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>211010</v>
+        <v>190968</v>
       </c>
       <c r="B64" t="str">
         <v>General Surgery</v>
@@ -1673,7 +1673,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D64" t="str">
-        <v>11:41:58</v>
+        <v>11:42:09</v>
       </c>
       <c r="E64" t="str">
         <v>Manual</v>
@@ -1684,7 +1684,7 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>190968</v>
+        <v>200933</v>
       </c>
       <c r="B65" t="str">
         <v>General Surgery</v>
@@ -1693,7 +1693,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D65" t="str">
-        <v>11:42:09</v>
+        <v>11:42:20</v>
       </c>
       <c r="E65" t="str">
         <v>Manual</v>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>200933</v>
+        <v>201825</v>
       </c>
       <c r="B66" t="str">
         <v>General Surgery</v>
@@ -1713,7 +1713,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D66" t="str">
-        <v>11:42:20</v>
+        <v>11:42:35</v>
       </c>
       <c r="E66" t="str">
         <v>Manual</v>
@@ -1724,7 +1724,7 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>201825</v>
+        <v>190801</v>
       </c>
       <c r="B67" t="str">
         <v>General Surgery</v>
@@ -1733,7 +1733,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D67" t="str">
-        <v>11:42:35</v>
+        <v>11:42:42</v>
       </c>
       <c r="E67" t="str">
         <v>Manual</v>
@@ -1744,7 +1744,7 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>190801</v>
+        <v>201465</v>
       </c>
       <c r="B68" t="str">
         <v>General Surgery</v>
@@ -1753,10 +1753,10 @@
         <v>11/10/2025</v>
       </c>
       <c r="D68" t="str">
-        <v>11:42:42</v>
+        <v>11:42:49</v>
       </c>
       <c r="E68" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F68" t="str">
         <v>dnasr281@gmail.com</v>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>201465</v>
+        <v>201171</v>
       </c>
       <c r="B69" t="str">
         <v>General Surgery</v>
@@ -1773,7 +1773,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D69" t="str">
-        <v>11:42:49</v>
+        <v>11:42:52</v>
       </c>
       <c r="E69" t="str">
         <v>Scan</v>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>201171</v>
+        <v>200491</v>
       </c>
       <c r="B70" t="str">
         <v>General Surgery</v>
@@ -1793,7 +1793,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D70" t="str">
-        <v>11:42:52</v>
+        <v>11:42:54</v>
       </c>
       <c r="E70" t="str">
         <v>Scan</v>
@@ -1804,7 +1804,7 @@
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>200491</v>
+        <v>200490</v>
       </c>
       <c r="B71" t="str">
         <v>General Surgery</v>
@@ -1813,7 +1813,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D71" t="str">
-        <v>11:42:54</v>
+        <v>11:42:56</v>
       </c>
       <c r="E71" t="str">
         <v>Scan</v>
@@ -1824,7 +1824,7 @@
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>200490</v>
+        <v>200228</v>
       </c>
       <c r="B72" t="str">
         <v>General Surgery</v>
@@ -1833,7 +1833,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D72" t="str">
-        <v>11:42:56</v>
+        <v>11:42:59</v>
       </c>
       <c r="E72" t="str">
         <v>Scan</v>
@@ -1844,7 +1844,7 @@
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>200228</v>
+        <v>201669</v>
       </c>
       <c r="B73" t="str">
         <v>General Surgery</v>
@@ -1853,7 +1853,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D73" t="str">
-        <v>11:42:59</v>
+        <v>11:43:01</v>
       </c>
       <c r="E73" t="str">
         <v>Scan</v>
@@ -1864,7 +1864,7 @@
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>201669</v>
+        <v>202004</v>
       </c>
       <c r="B74" t="str">
         <v>General Surgery</v>
@@ -1873,7 +1873,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D74" t="str">
-        <v>11:43:01</v>
+        <v>11:43:03</v>
       </c>
       <c r="E74" t="str">
         <v>Scan</v>
@@ -1884,7 +1884,7 @@
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>202004</v>
+        <v>200116</v>
       </c>
       <c r="B75" t="str">
         <v>General Surgery</v>
@@ -1893,7 +1893,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D75" t="str">
-        <v>11:43:03</v>
+        <v>11:43:05</v>
       </c>
       <c r="E75" t="str">
         <v>Scan</v>
@@ -1904,7 +1904,7 @@
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>200116</v>
+        <v>190796</v>
       </c>
       <c r="B76" t="str">
         <v>General Surgery</v>
@@ -1913,7 +1913,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D76" t="str">
-        <v>11:43:05</v>
+        <v>11:43:07</v>
       </c>
       <c r="E76" t="str">
         <v>Scan</v>
@@ -1924,7 +1924,7 @@
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>190796</v>
+        <v>190981</v>
       </c>
       <c r="B77" t="str">
         <v>General Surgery</v>
@@ -1933,7 +1933,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D77" t="str">
-        <v>11:43:07</v>
+        <v>11:43:09</v>
       </c>
       <c r="E77" t="str">
         <v>Scan</v>
@@ -1944,7 +1944,7 @@
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>190981</v>
+        <v>200163</v>
       </c>
       <c r="B78" t="str">
         <v>General Surgery</v>
@@ -1953,7 +1953,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D78" t="str">
-        <v>11:43:09</v>
+        <v>11:43:12</v>
       </c>
       <c r="E78" t="str">
         <v>Scan</v>
@@ -1964,7 +1964,7 @@
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>200163</v>
+        <v>191061</v>
       </c>
       <c r="B79" t="str">
         <v>General Surgery</v>
@@ -1973,7 +1973,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D79" t="str">
-        <v>11:43:12</v>
+        <v>11:43:15</v>
       </c>
       <c r="E79" t="str">
         <v>Scan</v>
@@ -1984,7 +1984,7 @@
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>191061</v>
+        <v>200744</v>
       </c>
       <c r="B80" t="str">
         <v>General Surgery</v>
@@ -1993,7 +1993,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D80" t="str">
-        <v>11:43:15</v>
+        <v>11:43:17</v>
       </c>
       <c r="E80" t="str">
         <v>Scan</v>
@@ -2004,7 +2004,7 @@
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>200744</v>
+        <v>201564</v>
       </c>
       <c r="B81" t="str">
         <v>General Surgery</v>
@@ -2013,7 +2013,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D81" t="str">
-        <v>11:43:17</v>
+        <v>11:43:20</v>
       </c>
       <c r="E81" t="str">
         <v>Scan</v>
@@ -2024,7 +2024,7 @@
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>201564</v>
+        <v>200804</v>
       </c>
       <c r="B82" t="str">
         <v>General Surgery</v>
@@ -2033,7 +2033,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D82" t="str">
-        <v>11:43:20</v>
+        <v>11:43:22</v>
       </c>
       <c r="E82" t="str">
         <v>Scan</v>
@@ -2044,7 +2044,7 @@
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>200804</v>
+        <v>200792</v>
       </c>
       <c r="B83" t="str">
         <v>General Surgery</v>
@@ -2053,7 +2053,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D83" t="str">
-        <v>11:43:22</v>
+        <v>11:43:24</v>
       </c>
       <c r="E83" t="str">
         <v>Scan</v>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>200792</v>
+        <v>200628</v>
       </c>
       <c r="B84" t="str">
         <v>General Surgery</v>
@@ -2073,7 +2073,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D84" t="str">
-        <v>11:43:24</v>
+        <v>11:43:26</v>
       </c>
       <c r="E84" t="str">
         <v>Scan</v>
@@ -2084,7 +2084,7 @@
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>200628</v>
+        <v>211216</v>
       </c>
       <c r="B85" t="str">
         <v>General Surgery</v>
@@ -2093,7 +2093,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D85" t="str">
-        <v>11:43:26</v>
+        <v>11:43:28</v>
       </c>
       <c r="E85" t="str">
         <v>Scan</v>
@@ -2104,7 +2104,7 @@
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>211216</v>
+        <v>211197</v>
       </c>
       <c r="B86" t="str">
         <v>General Surgery</v>
@@ -2113,7 +2113,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D86" t="str">
-        <v>11:43:28</v>
+        <v>11:43:31</v>
       </c>
       <c r="E86" t="str">
         <v>Scan</v>
@@ -2124,7 +2124,7 @@
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>211197</v>
+        <v>201397</v>
       </c>
       <c r="B87" t="str">
         <v>General Surgery</v>
@@ -2133,7 +2133,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D87" t="str">
-        <v>11:43:31</v>
+        <v>11:43:33</v>
       </c>
       <c r="E87" t="str">
         <v>Scan</v>
@@ -2144,7 +2144,7 @@
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>201397</v>
+        <v>200917</v>
       </c>
       <c r="B88" t="str">
         <v>General Surgery</v>
@@ -2153,7 +2153,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D88" t="str">
-        <v>11:43:33</v>
+        <v>11:43:35</v>
       </c>
       <c r="E88" t="str">
         <v>Scan</v>
@@ -2164,7 +2164,7 @@
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>200917</v>
+        <v>201051</v>
       </c>
       <c r="B89" t="str">
         <v>General Surgery</v>
@@ -2173,7 +2173,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D89" t="str">
-        <v>11:43:35</v>
+        <v>11:43:37</v>
       </c>
       <c r="E89" t="str">
         <v>Scan</v>
@@ -2184,7 +2184,7 @@
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>201051</v>
+        <v>201501</v>
       </c>
       <c r="B90" t="str">
         <v>General Surgery</v>
@@ -2193,7 +2193,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D90" t="str">
-        <v>11:43:37</v>
+        <v>11:43:40</v>
       </c>
       <c r="E90" t="str">
         <v>Scan</v>
@@ -2204,7 +2204,7 @@
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>201501</v>
+        <v>200905</v>
       </c>
       <c r="B91" t="str">
         <v>General Surgery</v>
@@ -2213,7 +2213,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D91" t="str">
-        <v>11:43:40</v>
+        <v>11:43:42</v>
       </c>
       <c r="E91" t="str">
         <v>Scan</v>
@@ -2224,7 +2224,7 @@
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>200905</v>
+        <v>200938</v>
       </c>
       <c r="B92" t="str">
         <v>General Surgery</v>
@@ -2233,7 +2233,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D92" t="str">
-        <v>11:43:42</v>
+        <v>11:43:45</v>
       </c>
       <c r="E92" t="str">
         <v>Scan</v>
@@ -2244,7 +2244,7 @@
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>200938</v>
+        <v>211043</v>
       </c>
       <c r="B93" t="str">
         <v>General Surgery</v>
@@ -2253,7 +2253,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D93" t="str">
-        <v>11:43:45</v>
+        <v>11:43:47</v>
       </c>
       <c r="E93" t="str">
         <v>Scan</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>211043</v>
+        <v>211133</v>
       </c>
       <c r="B94" t="str">
         <v>General Surgery</v>
@@ -2273,7 +2273,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D94" t="str">
-        <v>11:43:47</v>
+        <v>11:43:49</v>
       </c>
       <c r="E94" t="str">
         <v>Scan</v>
@@ -2284,7 +2284,7 @@
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>211133</v>
+        <v>211741</v>
       </c>
       <c r="B95" t="str">
         <v>General Surgery</v>
@@ -2293,7 +2293,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D95" t="str">
-        <v>11:43:49</v>
+        <v>11:43:50</v>
       </c>
       <c r="E95" t="str">
         <v>Scan</v>
@@ -2304,7 +2304,7 @@
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>211741</v>
+        <v>211245</v>
       </c>
       <c r="B96" t="str">
         <v>General Surgery</v>
@@ -2313,7 +2313,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D96" t="str">
-        <v>11:43:50</v>
+        <v>11:43:52</v>
       </c>
       <c r="E96" t="str">
         <v>Scan</v>
@@ -2324,7 +2324,7 @@
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>211245</v>
+        <v>190929</v>
       </c>
       <c r="B97" t="str">
         <v>General Surgery</v>
@@ -2333,7 +2333,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D97" t="str">
-        <v>11:43:52</v>
+        <v>11:43:55</v>
       </c>
       <c r="E97" t="str">
         <v>Scan</v>
@@ -2344,7 +2344,7 @@
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>190929</v>
+        <v>191119</v>
       </c>
       <c r="B98" t="str">
         <v>General Surgery</v>
@@ -2353,7 +2353,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D98" t="str">
-        <v>11:43:55</v>
+        <v>11:43:56</v>
       </c>
       <c r="E98" t="str">
         <v>Scan</v>
@@ -2364,7 +2364,7 @@
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>191119</v>
+        <v>211210</v>
       </c>
       <c r="B99" t="str">
         <v>General Surgery</v>
@@ -2373,10 +2373,10 @@
         <v>11/10/2025</v>
       </c>
       <c r="D99" t="str">
-        <v>11:43:56</v>
+        <v>11:44:43</v>
       </c>
       <c r="E99" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F99" t="str">
         <v>dnasr281@gmail.com</v>
@@ -2384,7 +2384,7 @@
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>211210</v>
+        <v>201880</v>
       </c>
       <c r="B100" t="str">
         <v>General Surgery</v>
@@ -2393,7 +2393,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D100" t="str">
-        <v>11:44:43</v>
+        <v>11:45:28</v>
       </c>
       <c r="E100" t="str">
         <v>Manual</v>
@@ -2404,7 +2404,7 @@
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>201880</v>
+        <v>211246</v>
       </c>
       <c r="B101" t="str">
         <v>General Surgery</v>
@@ -2413,7 +2413,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D101" t="str">
-        <v>11:45:28</v>
+        <v>11:45:59</v>
       </c>
       <c r="E101" t="str">
         <v>Manual</v>
@@ -2424,7 +2424,7 @@
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>211246</v>
+        <v>201823</v>
       </c>
       <c r="B102" t="str">
         <v>General Surgery</v>
@@ -2433,7 +2433,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D102" t="str">
-        <v>11:45:59</v>
+        <v>11:46:33</v>
       </c>
       <c r="E102" t="str">
         <v>Manual</v>
@@ -2444,7 +2444,7 @@
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>201823</v>
+        <v>200928</v>
       </c>
       <c r="B103" t="str">
         <v>General Surgery</v>
@@ -2453,7 +2453,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D103" t="str">
-        <v>11:46:33</v>
+        <v>11:47:11</v>
       </c>
       <c r="E103" t="str">
         <v>Manual</v>
@@ -2464,7 +2464,7 @@
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>200928</v>
+        <v>201237</v>
       </c>
       <c r="B104" t="str">
         <v>General Surgery</v>
@@ -2473,7 +2473,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D104" t="str">
-        <v>11:47:11</v>
+        <v>11:47:35</v>
       </c>
       <c r="E104" t="str">
         <v>Manual</v>
@@ -2484,7 +2484,7 @@
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>201237</v>
+        <v>201513</v>
       </c>
       <c r="B105" t="str">
         <v>General Surgery</v>
@@ -2493,7 +2493,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D105" t="str">
-        <v>11:47:35</v>
+        <v>11:48:02</v>
       </c>
       <c r="E105" t="str">
         <v>Manual</v>
@@ -2504,7 +2504,7 @@
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>201513</v>
+        <v>200997</v>
       </c>
       <c r="B106" t="str">
         <v>General Surgery</v>
@@ -2513,7 +2513,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D106" t="str">
-        <v>11:48:02</v>
+        <v>11:48:26</v>
       </c>
       <c r="E106" t="str">
         <v>Manual</v>
@@ -2524,7 +2524,7 @@
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>200997</v>
+        <v>181004</v>
       </c>
       <c r="B107" t="str">
         <v>General Surgery</v>
@@ -2533,7 +2533,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D107" t="str">
-        <v>11:48:26</v>
+        <v>11:48:49</v>
       </c>
       <c r="E107" t="str">
         <v>Manual</v>
@@ -2544,7 +2544,7 @@
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>181004</v>
+        <v>211121</v>
       </c>
       <c r="B108" t="str">
         <v>General Surgery</v>
@@ -2553,7 +2553,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D108" t="str">
-        <v>11:48:49</v>
+        <v>11:49:14</v>
       </c>
       <c r="E108" t="str">
         <v>Manual</v>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>211121</v>
+        <v>201252</v>
       </c>
       <c r="B109" t="str">
         <v>General Surgery</v>
@@ -2573,7 +2573,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D109" t="str">
-        <v>11:49:14</v>
+        <v>11:49:29</v>
       </c>
       <c r="E109" t="str">
         <v>Manual</v>
@@ -2584,7 +2584,7 @@
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>201252</v>
+        <v>201023</v>
       </c>
       <c r="B110" t="str">
         <v>General Surgery</v>
@@ -2593,7 +2593,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D110" t="str">
-        <v>11:49:29</v>
+        <v>11:49:42</v>
       </c>
       <c r="E110" t="str">
         <v>Manual</v>
@@ -2604,7 +2604,7 @@
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>201023</v>
+        <v>201253</v>
       </c>
       <c r="B111" t="str">
         <v>General Surgery</v>
@@ -2613,7 +2613,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D111" t="str">
-        <v>11:49:42</v>
+        <v>11:49:57</v>
       </c>
       <c r="E111" t="str">
         <v>Manual</v>
@@ -2624,7 +2624,7 @@
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>201253</v>
+        <v>201337</v>
       </c>
       <c r="B112" t="str">
         <v>General Surgery</v>
@@ -2633,7 +2633,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D112" t="str">
-        <v>11:49:57</v>
+        <v>11:50:11</v>
       </c>
       <c r="E112" t="str">
         <v>Manual</v>
@@ -2644,7 +2644,7 @@
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>201337</v>
+        <v>201572</v>
       </c>
       <c r="B113" t="str">
         <v>General Surgery</v>
@@ -2653,10 +2653,10 @@
         <v>11/10/2025</v>
       </c>
       <c r="D113" t="str">
-        <v>11:50:11</v>
+        <v>11:50:20</v>
       </c>
       <c r="E113" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F113" t="str">
         <v>dnasr281@gmail.com</v>
@@ -2664,7 +2664,7 @@
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>201572</v>
+        <v>201398</v>
       </c>
       <c r="B114" t="str">
         <v>General Surgery</v>
@@ -2673,38 +2673,18 @@
         <v>11/10/2025</v>
       </c>
       <c r="D114" t="str">
-        <v>11:50:20</v>
+        <v>11:50:41</v>
       </c>
       <c r="E114" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F114" t="str">
-        <v>dnasr281@gmail.com</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="str">
-        <v>201398</v>
-      </c>
-      <c r="B115" t="str">
-        <v>General Surgery</v>
-      </c>
-      <c r="C115" t="str">
-        <v>11/10/2025</v>
-      </c>
-      <c r="D115" t="str">
-        <v>11:50:41</v>
-      </c>
-      <c r="E115" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F115" t="str">
         <v>dnasr281@gmail.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F115"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F114"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update edited session - 2025-10-11T10:30:12.698Z - Cache Bust ID: 1760178612698v72fjjrlq
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_General_Surgery_scanner1760170816881_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
+++ b/log_history/Y4_B2526_General_Surgery_scanner1760170816881_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="General_Surgery" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F114"/>
+  <dimension ref="A1:F113"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1204,7 +1204,7 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>201834</v>
+        <v>211118</v>
       </c>
       <c r="B41" t="str">
         <v>General Surgery</v>
@@ -1213,7 +1213,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D41" t="str">
-        <v>11:35:22</v>
+        <v>11:36:25</v>
       </c>
       <c r="E41" t="str">
         <v>Manual</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>211118</v>
+        <v>200904</v>
       </c>
       <c r="B42" t="str">
         <v>General Surgery</v>
@@ -1233,7 +1233,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D42" t="str">
-        <v>11:36:25</v>
+        <v>11:37:01</v>
       </c>
       <c r="E42" t="str">
         <v>Manual</v>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>200904</v>
+        <v>201632</v>
       </c>
       <c r="B43" t="str">
         <v>General Surgery</v>
@@ -1253,7 +1253,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D43" t="str">
-        <v>11:37:01</v>
+        <v>11:37:08</v>
       </c>
       <c r="E43" t="str">
         <v>Manual</v>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>201632</v>
+        <v>201190</v>
       </c>
       <c r="B44" t="str">
         <v>General Surgery</v>
@@ -1273,7 +1273,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D44" t="str">
-        <v>11:37:08</v>
+        <v>11:37:15</v>
       </c>
       <c r="E44" t="str">
         <v>Manual</v>
@@ -1284,7 +1284,7 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>201190</v>
+        <v>200824</v>
       </c>
       <c r="B45" t="str">
         <v>General Surgery</v>
@@ -1293,7 +1293,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D45" t="str">
-        <v>11:37:15</v>
+        <v>11:37:21</v>
       </c>
       <c r="E45" t="str">
         <v>Manual</v>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>200824</v>
+        <v>201197</v>
       </c>
       <c r="B46" t="str">
         <v>General Surgery</v>
@@ -1313,7 +1313,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D46" t="str">
-        <v>11:37:21</v>
+        <v>11:37:28</v>
       </c>
       <c r="E46" t="str">
         <v>Manual</v>
@@ -1324,7 +1324,7 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>201197</v>
+        <v>200914</v>
       </c>
       <c r="B47" t="str">
         <v>General Surgery</v>
@@ -1333,7 +1333,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D47" t="str">
-        <v>11:37:28</v>
+        <v>11:37:39</v>
       </c>
       <c r="E47" t="str">
         <v>Manual</v>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>200914</v>
+        <v>201065</v>
       </c>
       <c r="B48" t="str">
         <v>General Surgery</v>
@@ -1353,7 +1353,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D48" t="str">
-        <v>11:37:39</v>
+        <v>11:38:11</v>
       </c>
       <c r="E48" t="str">
         <v>Manual</v>
@@ -1364,7 +1364,7 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>201065</v>
+        <v>191478</v>
       </c>
       <c r="B49" t="str">
         <v>General Surgery</v>
@@ -1373,7 +1373,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D49" t="str">
-        <v>11:38:11</v>
+        <v>11:38:32</v>
       </c>
       <c r="E49" t="str">
         <v>Manual</v>
@@ -1384,7 +1384,7 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>191478</v>
+        <v>200999</v>
       </c>
       <c r="B50" t="str">
         <v>General Surgery</v>
@@ -1393,7 +1393,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D50" t="str">
-        <v>11:38:32</v>
+        <v>11:38:40</v>
       </c>
       <c r="E50" t="str">
         <v>Manual</v>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>200999</v>
+        <v>201157</v>
       </c>
       <c r="B51" t="str">
         <v>General Surgery</v>
@@ -1413,7 +1413,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D51" t="str">
-        <v>11:38:40</v>
+        <v>11:38:51</v>
       </c>
       <c r="E51" t="str">
         <v>Manual</v>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>201157</v>
+        <v>190314</v>
       </c>
       <c r="B52" t="str">
         <v>General Surgery</v>
@@ -1433,7 +1433,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D52" t="str">
-        <v>11:38:51</v>
+        <v>11:39:02</v>
       </c>
       <c r="E52" t="str">
         <v>Manual</v>
@@ -1444,7 +1444,7 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>190314</v>
+        <v>202162</v>
       </c>
       <c r="B53" t="str">
         <v>General Surgery</v>
@@ -1453,7 +1453,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D53" t="str">
-        <v>11:39:02</v>
+        <v>11:39:12</v>
       </c>
       <c r="E53" t="str">
         <v>Manual</v>
@@ -1464,7 +1464,7 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>202162</v>
+        <v>201819</v>
       </c>
       <c r="B54" t="str">
         <v>General Surgery</v>
@@ -1473,7 +1473,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D54" t="str">
-        <v>11:39:12</v>
+        <v>11:39:21</v>
       </c>
       <c r="E54" t="str">
         <v>Manual</v>
@@ -1484,7 +1484,7 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>201819</v>
+        <v>201990</v>
       </c>
       <c r="B55" t="str">
         <v>General Surgery</v>
@@ -1493,7 +1493,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D55" t="str">
-        <v>11:39:21</v>
+        <v>11:39:29</v>
       </c>
       <c r="E55" t="str">
         <v>Manual</v>
@@ -1504,7 +1504,7 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>201990</v>
+        <v>211175</v>
       </c>
       <c r="B56" t="str">
         <v>General Surgery</v>
@@ -1513,7 +1513,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D56" t="str">
-        <v>11:39:29</v>
+        <v>11:39:42</v>
       </c>
       <c r="E56" t="str">
         <v>Manual</v>
@@ -1524,7 +1524,7 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>211175</v>
+        <v>201795</v>
       </c>
       <c r="B57" t="str">
         <v>General Surgery</v>
@@ -1533,7 +1533,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D57" t="str">
-        <v>11:39:42</v>
+        <v>11:39:58</v>
       </c>
       <c r="E57" t="str">
         <v>Manual</v>
@@ -1544,7 +1544,7 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>201795</v>
+        <v>211174</v>
       </c>
       <c r="B58" t="str">
         <v>General Surgery</v>
@@ -1553,7 +1553,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D58" t="str">
-        <v>11:39:58</v>
+        <v>11:41:21</v>
       </c>
       <c r="E58" t="str">
         <v>Manual</v>
@@ -1564,7 +1564,7 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>211174</v>
+        <v>211092</v>
       </c>
       <c r="B59" t="str">
         <v>General Surgery</v>
@@ -1573,7 +1573,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D59" t="str">
-        <v>11:41:21</v>
+        <v>11:41:29</v>
       </c>
       <c r="E59" t="str">
         <v>Manual</v>
@@ -1584,7 +1584,7 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>211092</v>
+        <v>211046</v>
       </c>
       <c r="B60" t="str">
         <v>General Surgery</v>
@@ -1593,7 +1593,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D60" t="str">
-        <v>11:41:29</v>
+        <v>11:41:38</v>
       </c>
       <c r="E60" t="str">
         <v>Manual</v>
@@ -1604,7 +1604,7 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>211046</v>
+        <v>211242</v>
       </c>
       <c r="B61" t="str">
         <v>General Surgery</v>
@@ -1613,7 +1613,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D61" t="str">
-        <v>11:41:38</v>
+        <v>11:41:50</v>
       </c>
       <c r="E61" t="str">
         <v>Manual</v>
@@ -1624,7 +1624,7 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>211242</v>
+        <v>211010</v>
       </c>
       <c r="B62" t="str">
         <v>General Surgery</v>
@@ -1633,7 +1633,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D62" t="str">
-        <v>11:41:50</v>
+        <v>11:41:58</v>
       </c>
       <c r="E62" t="str">
         <v>Manual</v>
@@ -1644,7 +1644,7 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>211010</v>
+        <v>190968</v>
       </c>
       <c r="B63" t="str">
         <v>General Surgery</v>
@@ -1653,7 +1653,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D63" t="str">
-        <v>11:41:58</v>
+        <v>11:42:09</v>
       </c>
       <c r="E63" t="str">
         <v>Manual</v>
@@ -1664,7 +1664,7 @@
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>190968</v>
+        <v>200933</v>
       </c>
       <c r="B64" t="str">
         <v>General Surgery</v>
@@ -1673,7 +1673,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D64" t="str">
-        <v>11:42:09</v>
+        <v>11:42:20</v>
       </c>
       <c r="E64" t="str">
         <v>Manual</v>
@@ -1684,7 +1684,7 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>200933</v>
+        <v>201825</v>
       </c>
       <c r="B65" t="str">
         <v>General Surgery</v>
@@ -1693,7 +1693,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D65" t="str">
-        <v>11:42:20</v>
+        <v>11:42:35</v>
       </c>
       <c r="E65" t="str">
         <v>Manual</v>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>201825</v>
+        <v>190801</v>
       </c>
       <c r="B66" t="str">
         <v>General Surgery</v>
@@ -1713,7 +1713,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D66" t="str">
-        <v>11:42:35</v>
+        <v>11:42:42</v>
       </c>
       <c r="E66" t="str">
         <v>Manual</v>
@@ -1724,7 +1724,7 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>190801</v>
+        <v>201465</v>
       </c>
       <c r="B67" t="str">
         <v>General Surgery</v>
@@ -1733,10 +1733,10 @@
         <v>11/10/2025</v>
       </c>
       <c r="D67" t="str">
-        <v>11:42:42</v>
+        <v>11:42:49</v>
       </c>
       <c r="E67" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F67" t="str">
         <v>dnasr281@gmail.com</v>
@@ -1744,7 +1744,7 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>201465</v>
+        <v>201171</v>
       </c>
       <c r="B68" t="str">
         <v>General Surgery</v>
@@ -1753,7 +1753,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D68" t="str">
-        <v>11:42:49</v>
+        <v>11:42:52</v>
       </c>
       <c r="E68" t="str">
         <v>Scan</v>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>201171</v>
+        <v>200491</v>
       </c>
       <c r="B69" t="str">
         <v>General Surgery</v>
@@ -1773,7 +1773,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D69" t="str">
-        <v>11:42:52</v>
+        <v>11:42:54</v>
       </c>
       <c r="E69" t="str">
         <v>Scan</v>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>200491</v>
+        <v>200490</v>
       </c>
       <c r="B70" t="str">
         <v>General Surgery</v>
@@ -1793,7 +1793,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D70" t="str">
-        <v>11:42:54</v>
+        <v>11:42:56</v>
       </c>
       <c r="E70" t="str">
         <v>Scan</v>
@@ -1804,7 +1804,7 @@
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>200490</v>
+        <v>200228</v>
       </c>
       <c r="B71" t="str">
         <v>General Surgery</v>
@@ -1813,7 +1813,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D71" t="str">
-        <v>11:42:56</v>
+        <v>11:42:59</v>
       </c>
       <c r="E71" t="str">
         <v>Scan</v>
@@ -1824,7 +1824,7 @@
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>200228</v>
+        <v>201669</v>
       </c>
       <c r="B72" t="str">
         <v>General Surgery</v>
@@ -1833,7 +1833,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D72" t="str">
-        <v>11:42:59</v>
+        <v>11:43:01</v>
       </c>
       <c r="E72" t="str">
         <v>Scan</v>
@@ -1844,7 +1844,7 @@
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>201669</v>
+        <v>202004</v>
       </c>
       <c r="B73" t="str">
         <v>General Surgery</v>
@@ -1853,7 +1853,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D73" t="str">
-        <v>11:43:01</v>
+        <v>11:43:03</v>
       </c>
       <c r="E73" t="str">
         <v>Scan</v>
@@ -1864,7 +1864,7 @@
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>202004</v>
+        <v>200116</v>
       </c>
       <c r="B74" t="str">
         <v>General Surgery</v>
@@ -1873,7 +1873,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D74" t="str">
-        <v>11:43:03</v>
+        <v>11:43:05</v>
       </c>
       <c r="E74" t="str">
         <v>Scan</v>
@@ -1884,7 +1884,7 @@
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>200116</v>
+        <v>190796</v>
       </c>
       <c r="B75" t="str">
         <v>General Surgery</v>
@@ -1893,7 +1893,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D75" t="str">
-        <v>11:43:05</v>
+        <v>11:43:07</v>
       </c>
       <c r="E75" t="str">
         <v>Scan</v>
@@ -1904,7 +1904,7 @@
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>190796</v>
+        <v>190981</v>
       </c>
       <c r="B76" t="str">
         <v>General Surgery</v>
@@ -1913,7 +1913,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D76" t="str">
-        <v>11:43:07</v>
+        <v>11:43:09</v>
       </c>
       <c r="E76" t="str">
         <v>Scan</v>
@@ -1924,7 +1924,7 @@
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>190981</v>
+        <v>200163</v>
       </c>
       <c r="B77" t="str">
         <v>General Surgery</v>
@@ -1933,7 +1933,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D77" t="str">
-        <v>11:43:09</v>
+        <v>11:43:12</v>
       </c>
       <c r="E77" t="str">
         <v>Scan</v>
@@ -1944,7 +1944,7 @@
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>200163</v>
+        <v>191061</v>
       </c>
       <c r="B78" t="str">
         <v>General Surgery</v>
@@ -1953,7 +1953,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D78" t="str">
-        <v>11:43:12</v>
+        <v>11:43:15</v>
       </c>
       <c r="E78" t="str">
         <v>Scan</v>
@@ -1964,7 +1964,7 @@
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>191061</v>
+        <v>200744</v>
       </c>
       <c r="B79" t="str">
         <v>General Surgery</v>
@@ -1973,7 +1973,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D79" t="str">
-        <v>11:43:15</v>
+        <v>11:43:17</v>
       </c>
       <c r="E79" t="str">
         <v>Scan</v>
@@ -1984,7 +1984,7 @@
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>200744</v>
+        <v>201564</v>
       </c>
       <c r="B80" t="str">
         <v>General Surgery</v>
@@ -1993,7 +1993,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D80" t="str">
-        <v>11:43:17</v>
+        <v>11:43:20</v>
       </c>
       <c r="E80" t="str">
         <v>Scan</v>
@@ -2004,7 +2004,7 @@
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>201564</v>
+        <v>200804</v>
       </c>
       <c r="B81" t="str">
         <v>General Surgery</v>
@@ -2013,7 +2013,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D81" t="str">
-        <v>11:43:20</v>
+        <v>11:43:22</v>
       </c>
       <c r="E81" t="str">
         <v>Scan</v>
@@ -2024,7 +2024,7 @@
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>200804</v>
+        <v>200792</v>
       </c>
       <c r="B82" t="str">
         <v>General Surgery</v>
@@ -2033,7 +2033,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D82" t="str">
-        <v>11:43:22</v>
+        <v>11:43:24</v>
       </c>
       <c r="E82" t="str">
         <v>Scan</v>
@@ -2044,7 +2044,7 @@
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>200792</v>
+        <v>200628</v>
       </c>
       <c r="B83" t="str">
         <v>General Surgery</v>
@@ -2053,7 +2053,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D83" t="str">
-        <v>11:43:24</v>
+        <v>11:43:26</v>
       </c>
       <c r="E83" t="str">
         <v>Scan</v>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>200628</v>
+        <v>211216</v>
       </c>
       <c r="B84" t="str">
         <v>General Surgery</v>
@@ -2073,7 +2073,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D84" t="str">
-        <v>11:43:26</v>
+        <v>11:43:28</v>
       </c>
       <c r="E84" t="str">
         <v>Scan</v>
@@ -2084,7 +2084,7 @@
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>211216</v>
+        <v>211197</v>
       </c>
       <c r="B85" t="str">
         <v>General Surgery</v>
@@ -2093,7 +2093,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D85" t="str">
-        <v>11:43:28</v>
+        <v>11:43:31</v>
       </c>
       <c r="E85" t="str">
         <v>Scan</v>
@@ -2104,7 +2104,7 @@
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>211197</v>
+        <v>201397</v>
       </c>
       <c r="B86" t="str">
         <v>General Surgery</v>
@@ -2113,7 +2113,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D86" t="str">
-        <v>11:43:31</v>
+        <v>11:43:33</v>
       </c>
       <c r="E86" t="str">
         <v>Scan</v>
@@ -2124,7 +2124,7 @@
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>201397</v>
+        <v>200917</v>
       </c>
       <c r="B87" t="str">
         <v>General Surgery</v>
@@ -2133,7 +2133,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D87" t="str">
-        <v>11:43:33</v>
+        <v>11:43:35</v>
       </c>
       <c r="E87" t="str">
         <v>Scan</v>
@@ -2144,7 +2144,7 @@
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>200917</v>
+        <v>201051</v>
       </c>
       <c r="B88" t="str">
         <v>General Surgery</v>
@@ -2153,7 +2153,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D88" t="str">
-        <v>11:43:35</v>
+        <v>11:43:37</v>
       </c>
       <c r="E88" t="str">
         <v>Scan</v>
@@ -2164,7 +2164,7 @@
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>201051</v>
+        <v>201501</v>
       </c>
       <c r="B89" t="str">
         <v>General Surgery</v>
@@ -2173,7 +2173,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D89" t="str">
-        <v>11:43:37</v>
+        <v>11:43:40</v>
       </c>
       <c r="E89" t="str">
         <v>Scan</v>
@@ -2184,7 +2184,7 @@
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>201501</v>
+        <v>200905</v>
       </c>
       <c r="B90" t="str">
         <v>General Surgery</v>
@@ -2193,7 +2193,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D90" t="str">
-        <v>11:43:40</v>
+        <v>11:43:42</v>
       </c>
       <c r="E90" t="str">
         <v>Scan</v>
@@ -2204,7 +2204,7 @@
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>200905</v>
+        <v>200938</v>
       </c>
       <c r="B91" t="str">
         <v>General Surgery</v>
@@ -2213,7 +2213,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D91" t="str">
-        <v>11:43:42</v>
+        <v>11:43:45</v>
       </c>
       <c r="E91" t="str">
         <v>Scan</v>
@@ -2224,7 +2224,7 @@
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>200938</v>
+        <v>211043</v>
       </c>
       <c r="B92" t="str">
         <v>General Surgery</v>
@@ -2233,7 +2233,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D92" t="str">
-        <v>11:43:45</v>
+        <v>11:43:47</v>
       </c>
       <c r="E92" t="str">
         <v>Scan</v>
@@ -2244,7 +2244,7 @@
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>211043</v>
+        <v>211133</v>
       </c>
       <c r="B93" t="str">
         <v>General Surgery</v>
@@ -2253,7 +2253,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D93" t="str">
-        <v>11:43:47</v>
+        <v>11:43:49</v>
       </c>
       <c r="E93" t="str">
         <v>Scan</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>211133</v>
+        <v>211741</v>
       </c>
       <c r="B94" t="str">
         <v>General Surgery</v>
@@ -2273,7 +2273,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D94" t="str">
-        <v>11:43:49</v>
+        <v>11:43:50</v>
       </c>
       <c r="E94" t="str">
         <v>Scan</v>
@@ -2284,7 +2284,7 @@
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>211741</v>
+        <v>211245</v>
       </c>
       <c r="B95" t="str">
         <v>General Surgery</v>
@@ -2293,7 +2293,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D95" t="str">
-        <v>11:43:50</v>
+        <v>11:43:52</v>
       </c>
       <c r="E95" t="str">
         <v>Scan</v>
@@ -2304,7 +2304,7 @@
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>211245</v>
+        <v>190929</v>
       </c>
       <c r="B96" t="str">
         <v>General Surgery</v>
@@ -2313,7 +2313,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D96" t="str">
-        <v>11:43:52</v>
+        <v>11:43:55</v>
       </c>
       <c r="E96" t="str">
         <v>Scan</v>
@@ -2324,7 +2324,7 @@
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>190929</v>
+        <v>191119</v>
       </c>
       <c r="B97" t="str">
         <v>General Surgery</v>
@@ -2333,7 +2333,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D97" t="str">
-        <v>11:43:55</v>
+        <v>11:43:56</v>
       </c>
       <c r="E97" t="str">
         <v>Scan</v>
@@ -2344,7 +2344,7 @@
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>191119</v>
+        <v>211210</v>
       </c>
       <c r="B98" t="str">
         <v>General Surgery</v>
@@ -2353,10 +2353,10 @@
         <v>11/10/2025</v>
       </c>
       <c r="D98" t="str">
-        <v>11:43:56</v>
+        <v>11:44:43</v>
       </c>
       <c r="E98" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F98" t="str">
         <v>dnasr281@gmail.com</v>
@@ -2364,7 +2364,7 @@
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>211210</v>
+        <v>201880</v>
       </c>
       <c r="B99" t="str">
         <v>General Surgery</v>
@@ -2373,7 +2373,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D99" t="str">
-        <v>11:44:43</v>
+        <v>11:45:28</v>
       </c>
       <c r="E99" t="str">
         <v>Manual</v>
@@ -2384,7 +2384,7 @@
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>201880</v>
+        <v>211246</v>
       </c>
       <c r="B100" t="str">
         <v>General Surgery</v>
@@ -2393,7 +2393,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D100" t="str">
-        <v>11:45:28</v>
+        <v>11:45:59</v>
       </c>
       <c r="E100" t="str">
         <v>Manual</v>
@@ -2404,7 +2404,7 @@
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>211246</v>
+        <v>201823</v>
       </c>
       <c r="B101" t="str">
         <v>General Surgery</v>
@@ -2413,7 +2413,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D101" t="str">
-        <v>11:45:59</v>
+        <v>11:46:33</v>
       </c>
       <c r="E101" t="str">
         <v>Manual</v>
@@ -2424,7 +2424,7 @@
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>201823</v>
+        <v>200928</v>
       </c>
       <c r="B102" t="str">
         <v>General Surgery</v>
@@ -2433,7 +2433,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D102" t="str">
-        <v>11:46:33</v>
+        <v>11:47:11</v>
       </c>
       <c r="E102" t="str">
         <v>Manual</v>
@@ -2444,7 +2444,7 @@
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>200928</v>
+        <v>201237</v>
       </c>
       <c r="B103" t="str">
         <v>General Surgery</v>
@@ -2453,7 +2453,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D103" t="str">
-        <v>11:47:11</v>
+        <v>11:47:35</v>
       </c>
       <c r="E103" t="str">
         <v>Manual</v>
@@ -2464,7 +2464,7 @@
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>201237</v>
+        <v>201513</v>
       </c>
       <c r="B104" t="str">
         <v>General Surgery</v>
@@ -2473,7 +2473,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D104" t="str">
-        <v>11:47:35</v>
+        <v>11:48:02</v>
       </c>
       <c r="E104" t="str">
         <v>Manual</v>
@@ -2484,7 +2484,7 @@
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>201513</v>
+        <v>200997</v>
       </c>
       <c r="B105" t="str">
         <v>General Surgery</v>
@@ -2493,7 +2493,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D105" t="str">
-        <v>11:48:02</v>
+        <v>11:48:26</v>
       </c>
       <c r="E105" t="str">
         <v>Manual</v>
@@ -2504,7 +2504,7 @@
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>200997</v>
+        <v>181004</v>
       </c>
       <c r="B106" t="str">
         <v>General Surgery</v>
@@ -2513,7 +2513,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D106" t="str">
-        <v>11:48:26</v>
+        <v>11:48:49</v>
       </c>
       <c r="E106" t="str">
         <v>Manual</v>
@@ -2524,7 +2524,7 @@
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>181004</v>
+        <v>211121</v>
       </c>
       <c r="B107" t="str">
         <v>General Surgery</v>
@@ -2533,7 +2533,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D107" t="str">
-        <v>11:48:49</v>
+        <v>11:49:14</v>
       </c>
       <c r="E107" t="str">
         <v>Manual</v>
@@ -2544,7 +2544,7 @@
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>211121</v>
+        <v>201252</v>
       </c>
       <c r="B108" t="str">
         <v>General Surgery</v>
@@ -2553,7 +2553,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D108" t="str">
-        <v>11:49:14</v>
+        <v>11:49:29</v>
       </c>
       <c r="E108" t="str">
         <v>Manual</v>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>201252</v>
+        <v>201023</v>
       </c>
       <c r="B109" t="str">
         <v>General Surgery</v>
@@ -2573,7 +2573,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D109" t="str">
-        <v>11:49:29</v>
+        <v>11:49:42</v>
       </c>
       <c r="E109" t="str">
         <v>Manual</v>
@@ -2584,7 +2584,7 @@
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>201023</v>
+        <v>201253</v>
       </c>
       <c r="B110" t="str">
         <v>General Surgery</v>
@@ -2593,7 +2593,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D110" t="str">
-        <v>11:49:42</v>
+        <v>11:49:57</v>
       </c>
       <c r="E110" t="str">
         <v>Manual</v>
@@ -2604,7 +2604,7 @@
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>201253</v>
+        <v>201337</v>
       </c>
       <c r="B111" t="str">
         <v>General Surgery</v>
@@ -2613,7 +2613,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D111" t="str">
-        <v>11:49:57</v>
+        <v>11:50:11</v>
       </c>
       <c r="E111" t="str">
         <v>Manual</v>
@@ -2624,7 +2624,7 @@
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>201337</v>
+        <v>201572</v>
       </c>
       <c r="B112" t="str">
         <v>General Surgery</v>
@@ -2633,10 +2633,10 @@
         <v>11/10/2025</v>
       </c>
       <c r="D112" t="str">
-        <v>11:50:11</v>
+        <v>11:50:20</v>
       </c>
       <c r="E112" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F112" t="str">
         <v>dnasr281@gmail.com</v>
@@ -2644,7 +2644,7 @@
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>201572</v>
+        <v>201398</v>
       </c>
       <c r="B113" t="str">
         <v>General Surgery</v>
@@ -2653,38 +2653,18 @@
         <v>11/10/2025</v>
       </c>
       <c r="D113" t="str">
-        <v>11:50:20</v>
+        <v>11:50:41</v>
       </c>
       <c r="E113" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F113" t="str">
-        <v>dnasr281@gmail.com</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="str">
-        <v>201398</v>
-      </c>
-      <c r="B114" t="str">
-        <v>General Surgery</v>
-      </c>
-      <c r="C114" t="str">
-        <v>11/10/2025</v>
-      </c>
-      <c r="D114" t="str">
-        <v>11:50:41</v>
-      </c>
-      <c r="E114" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F114" t="str">
         <v>dnasr281@gmail.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F114"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F113"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update edited session - 2025-10-11T10:58:46.803Z - Cache Bust ID: 176018032680308heurvf3
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_General_Surgery_scanner1760170816881_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
+++ b/log_history/Y4_B2526_General_Surgery_scanner1760170816881_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F113"/>
+  <dimension ref="A1:F112"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -764,7 +764,7 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>201438</v>
+        <v>191186</v>
       </c>
       <c r="B19" t="str">
         <v>General Surgery</v>
@@ -773,7 +773,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D19" t="str">
-        <v>11:25:50</v>
+        <v>11:26:11</v>
       </c>
       <c r="E19" t="str">
         <v>Manual</v>
@@ -784,7 +784,7 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>191186</v>
+        <v>191258</v>
       </c>
       <c r="B20" t="str">
         <v>General Surgery</v>
@@ -793,7 +793,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D20" t="str">
-        <v>11:26:11</v>
+        <v>11:27:36</v>
       </c>
       <c r="E20" t="str">
         <v>Manual</v>
@@ -804,7 +804,7 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>191258</v>
+        <v>200742</v>
       </c>
       <c r="B21" t="str">
         <v>General Surgery</v>
@@ -813,7 +813,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D21" t="str">
-        <v>11:27:36</v>
+        <v>11:27:56</v>
       </c>
       <c r="E21" t="str">
         <v>Manual</v>
@@ -824,7 +824,7 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>200742</v>
+        <v>201563</v>
       </c>
       <c r="B22" t="str">
         <v>General Surgery</v>
@@ -833,7 +833,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D22" t="str">
-        <v>11:27:56</v>
+        <v>11:28:13</v>
       </c>
       <c r="E22" t="str">
         <v>Manual</v>
@@ -844,7 +844,7 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>201563</v>
+        <v>180804</v>
       </c>
       <c r="B23" t="str">
         <v>General Surgery</v>
@@ -853,7 +853,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D23" t="str">
-        <v>11:28:13</v>
+        <v>11:28:23</v>
       </c>
       <c r="E23" t="str">
         <v>Manual</v>
@@ -864,7 +864,7 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>180804</v>
+        <v>211167</v>
       </c>
       <c r="B24" t="str">
         <v>General Surgery</v>
@@ -873,7 +873,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D24" t="str">
-        <v>11:28:23</v>
+        <v>11:28:31</v>
       </c>
       <c r="E24" t="str">
         <v>Manual</v>
@@ -884,7 +884,7 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>211167</v>
+        <v>211169</v>
       </c>
       <c r="B25" t="str">
         <v>General Surgery</v>
@@ -893,7 +893,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D25" t="str">
-        <v>11:28:31</v>
+        <v>11:28:41</v>
       </c>
       <c r="E25" t="str">
         <v>Manual</v>
@@ -904,7 +904,7 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>211169</v>
+        <v>211079</v>
       </c>
       <c r="B26" t="str">
         <v>General Surgery</v>
@@ -913,7 +913,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D26" t="str">
-        <v>11:28:41</v>
+        <v>11:28:48</v>
       </c>
       <c r="E26" t="str">
         <v>Manual</v>
@@ -924,7 +924,7 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>211079</v>
+        <v>200468</v>
       </c>
       <c r="B27" t="str">
         <v>General Surgery</v>
@@ -933,7 +933,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D27" t="str">
-        <v>11:28:48</v>
+        <v>11:29:01</v>
       </c>
       <c r="E27" t="str">
         <v>Manual</v>
@@ -944,7 +944,7 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>200468</v>
+        <v>191109</v>
       </c>
       <c r="B28" t="str">
         <v>General Surgery</v>
@@ -953,7 +953,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D28" t="str">
-        <v>11:29:01</v>
+        <v>11:29:08</v>
       </c>
       <c r="E28" t="str">
         <v>Manual</v>
@@ -964,7 +964,7 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>191109</v>
+        <v>191088</v>
       </c>
       <c r="B29" t="str">
         <v>General Surgery</v>
@@ -973,7 +973,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D29" t="str">
-        <v>11:29:08</v>
+        <v>11:29:17</v>
       </c>
       <c r="E29" t="str">
         <v>Manual</v>
@@ -984,7 +984,7 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>191088</v>
+        <v>200423</v>
       </c>
       <c r="B30" t="str">
         <v>General Surgery</v>
@@ -993,7 +993,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D30" t="str">
-        <v>11:29:17</v>
+        <v>11:29:25</v>
       </c>
       <c r="E30" t="str">
         <v>Manual</v>
@@ -1004,7 +1004,7 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>200423</v>
+        <v>190931</v>
       </c>
       <c r="B31" t="str">
         <v>General Surgery</v>
@@ -1013,7 +1013,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D31" t="str">
-        <v>11:29:25</v>
+        <v>11:29:35</v>
       </c>
       <c r="E31" t="str">
         <v>Manual</v>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>190931</v>
+        <v>190922</v>
       </c>
       <c r="B32" t="str">
         <v>General Surgery</v>
@@ -1033,7 +1033,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D32" t="str">
-        <v>11:29:35</v>
+        <v>11:29:50</v>
       </c>
       <c r="E32" t="str">
         <v>Manual</v>
@@ -1044,7 +1044,7 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>190922</v>
+        <v>191131</v>
       </c>
       <c r="B33" t="str">
         <v>General Surgery</v>
@@ -1053,7 +1053,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D33" t="str">
-        <v>11:29:50</v>
+        <v>11:30:02</v>
       </c>
       <c r="E33" t="str">
         <v>Manual</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>191131</v>
+        <v>190803</v>
       </c>
       <c r="B34" t="str">
         <v>General Surgery</v>
@@ -1073,7 +1073,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D34" t="str">
-        <v>11:30:02</v>
+        <v>11:30:15</v>
       </c>
       <c r="E34" t="str">
         <v>Manual</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>190803</v>
+        <v>181013</v>
       </c>
       <c r="B35" t="str">
         <v>General Surgery</v>
@@ -1093,7 +1093,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D35" t="str">
-        <v>11:30:15</v>
+        <v>11:30:22</v>
       </c>
       <c r="E35" t="str">
         <v>Manual</v>
@@ -1104,7 +1104,7 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>181013</v>
+        <v>201495</v>
       </c>
       <c r="B36" t="str">
         <v>General Surgery</v>
@@ -1113,7 +1113,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D36" t="str">
-        <v>11:30:22</v>
+        <v>11:30:50</v>
       </c>
       <c r="E36" t="str">
         <v>Manual</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>201495</v>
+        <v>201026</v>
       </c>
       <c r="B37" t="str">
         <v>General Surgery</v>
@@ -1133,7 +1133,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D37" t="str">
-        <v>11:30:50</v>
+        <v>11:33:15</v>
       </c>
       <c r="E37" t="str">
         <v>Manual</v>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>201026</v>
+        <v>200850</v>
       </c>
       <c r="B38" t="str">
         <v>General Surgery</v>
@@ -1153,7 +1153,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D38" t="str">
-        <v>11:33:15</v>
+        <v>11:33:26</v>
       </c>
       <c r="E38" t="str">
         <v>Manual</v>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>200850</v>
+        <v>200866</v>
       </c>
       <c r="B39" t="str">
         <v>General Surgery</v>
@@ -1173,7 +1173,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D39" t="str">
-        <v>11:33:26</v>
+        <v>11:33:36</v>
       </c>
       <c r="E39" t="str">
         <v>Manual</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>200866</v>
+        <v>211118</v>
       </c>
       <c r="B40" t="str">
         <v>General Surgery</v>
@@ -1193,7 +1193,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D40" t="str">
-        <v>11:33:36</v>
+        <v>11:36:25</v>
       </c>
       <c r="E40" t="str">
         <v>Manual</v>
@@ -1204,7 +1204,7 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>211118</v>
+        <v>200904</v>
       </c>
       <c r="B41" t="str">
         <v>General Surgery</v>
@@ -1213,7 +1213,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D41" t="str">
-        <v>11:36:25</v>
+        <v>11:37:01</v>
       </c>
       <c r="E41" t="str">
         <v>Manual</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>200904</v>
+        <v>201632</v>
       </c>
       <c r="B42" t="str">
         <v>General Surgery</v>
@@ -1233,7 +1233,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D42" t="str">
-        <v>11:37:01</v>
+        <v>11:37:08</v>
       </c>
       <c r="E42" t="str">
         <v>Manual</v>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>201632</v>
+        <v>201190</v>
       </c>
       <c r="B43" t="str">
         <v>General Surgery</v>
@@ -1253,7 +1253,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D43" t="str">
-        <v>11:37:08</v>
+        <v>11:37:15</v>
       </c>
       <c r="E43" t="str">
         <v>Manual</v>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>201190</v>
+        <v>200824</v>
       </c>
       <c r="B44" t="str">
         <v>General Surgery</v>
@@ -1273,7 +1273,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D44" t="str">
-        <v>11:37:15</v>
+        <v>11:37:21</v>
       </c>
       <c r="E44" t="str">
         <v>Manual</v>
@@ -1284,7 +1284,7 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>200824</v>
+        <v>201197</v>
       </c>
       <c r="B45" t="str">
         <v>General Surgery</v>
@@ -1293,7 +1293,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D45" t="str">
-        <v>11:37:21</v>
+        <v>11:37:28</v>
       </c>
       <c r="E45" t="str">
         <v>Manual</v>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>201197</v>
+        <v>200914</v>
       </c>
       <c r="B46" t="str">
         <v>General Surgery</v>
@@ -1313,7 +1313,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D46" t="str">
-        <v>11:37:28</v>
+        <v>11:37:39</v>
       </c>
       <c r="E46" t="str">
         <v>Manual</v>
@@ -1324,7 +1324,7 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>200914</v>
+        <v>201065</v>
       </c>
       <c r="B47" t="str">
         <v>General Surgery</v>
@@ -1333,7 +1333,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D47" t="str">
-        <v>11:37:39</v>
+        <v>11:38:11</v>
       </c>
       <c r="E47" t="str">
         <v>Manual</v>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>201065</v>
+        <v>191478</v>
       </c>
       <c r="B48" t="str">
         <v>General Surgery</v>
@@ -1353,7 +1353,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D48" t="str">
-        <v>11:38:11</v>
+        <v>11:38:32</v>
       </c>
       <c r="E48" t="str">
         <v>Manual</v>
@@ -1364,7 +1364,7 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>191478</v>
+        <v>200999</v>
       </c>
       <c r="B49" t="str">
         <v>General Surgery</v>
@@ -1373,7 +1373,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D49" t="str">
-        <v>11:38:32</v>
+        <v>11:38:40</v>
       </c>
       <c r="E49" t="str">
         <v>Manual</v>
@@ -1384,7 +1384,7 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>200999</v>
+        <v>201157</v>
       </c>
       <c r="B50" t="str">
         <v>General Surgery</v>
@@ -1393,7 +1393,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D50" t="str">
-        <v>11:38:40</v>
+        <v>11:38:51</v>
       </c>
       <c r="E50" t="str">
         <v>Manual</v>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>201157</v>
+        <v>190314</v>
       </c>
       <c r="B51" t="str">
         <v>General Surgery</v>
@@ -1413,7 +1413,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D51" t="str">
-        <v>11:38:51</v>
+        <v>11:39:02</v>
       </c>
       <c r="E51" t="str">
         <v>Manual</v>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>190314</v>
+        <v>202162</v>
       </c>
       <c r="B52" t="str">
         <v>General Surgery</v>
@@ -1433,7 +1433,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D52" t="str">
-        <v>11:39:02</v>
+        <v>11:39:12</v>
       </c>
       <c r="E52" t="str">
         <v>Manual</v>
@@ -1444,7 +1444,7 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>202162</v>
+        <v>201819</v>
       </c>
       <c r="B53" t="str">
         <v>General Surgery</v>
@@ -1453,7 +1453,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D53" t="str">
-        <v>11:39:12</v>
+        <v>11:39:21</v>
       </c>
       <c r="E53" t="str">
         <v>Manual</v>
@@ -1464,7 +1464,7 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>201819</v>
+        <v>201990</v>
       </c>
       <c r="B54" t="str">
         <v>General Surgery</v>
@@ -1473,7 +1473,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D54" t="str">
-        <v>11:39:21</v>
+        <v>11:39:29</v>
       </c>
       <c r="E54" t="str">
         <v>Manual</v>
@@ -1484,7 +1484,7 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>201990</v>
+        <v>211175</v>
       </c>
       <c r="B55" t="str">
         <v>General Surgery</v>
@@ -1493,7 +1493,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D55" t="str">
-        <v>11:39:29</v>
+        <v>11:39:42</v>
       </c>
       <c r="E55" t="str">
         <v>Manual</v>
@@ -1504,7 +1504,7 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>211175</v>
+        <v>201795</v>
       </c>
       <c r="B56" t="str">
         <v>General Surgery</v>
@@ -1513,7 +1513,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D56" t="str">
-        <v>11:39:42</v>
+        <v>11:39:58</v>
       </c>
       <c r="E56" t="str">
         <v>Manual</v>
@@ -1524,7 +1524,7 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>201795</v>
+        <v>211174</v>
       </c>
       <c r="B57" t="str">
         <v>General Surgery</v>
@@ -1533,7 +1533,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D57" t="str">
-        <v>11:39:58</v>
+        <v>11:41:21</v>
       </c>
       <c r="E57" t="str">
         <v>Manual</v>
@@ -1544,7 +1544,7 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>211174</v>
+        <v>211092</v>
       </c>
       <c r="B58" t="str">
         <v>General Surgery</v>
@@ -1553,7 +1553,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D58" t="str">
-        <v>11:41:21</v>
+        <v>11:41:29</v>
       </c>
       <c r="E58" t="str">
         <v>Manual</v>
@@ -1564,7 +1564,7 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>211092</v>
+        <v>211046</v>
       </c>
       <c r="B59" t="str">
         <v>General Surgery</v>
@@ -1573,7 +1573,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D59" t="str">
-        <v>11:41:29</v>
+        <v>11:41:38</v>
       </c>
       <c r="E59" t="str">
         <v>Manual</v>
@@ -1584,7 +1584,7 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>211046</v>
+        <v>211242</v>
       </c>
       <c r="B60" t="str">
         <v>General Surgery</v>
@@ -1593,7 +1593,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D60" t="str">
-        <v>11:41:38</v>
+        <v>11:41:50</v>
       </c>
       <c r="E60" t="str">
         <v>Manual</v>
@@ -1604,7 +1604,7 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>211242</v>
+        <v>211010</v>
       </c>
       <c r="B61" t="str">
         <v>General Surgery</v>
@@ -1613,7 +1613,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D61" t="str">
-        <v>11:41:50</v>
+        <v>11:41:58</v>
       </c>
       <c r="E61" t="str">
         <v>Manual</v>
@@ -1624,7 +1624,7 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>211010</v>
+        <v>190968</v>
       </c>
       <c r="B62" t="str">
         <v>General Surgery</v>
@@ -1633,7 +1633,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D62" t="str">
-        <v>11:41:58</v>
+        <v>11:42:09</v>
       </c>
       <c r="E62" t="str">
         <v>Manual</v>
@@ -1644,7 +1644,7 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>190968</v>
+        <v>200933</v>
       </c>
       <c r="B63" t="str">
         <v>General Surgery</v>
@@ -1653,7 +1653,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D63" t="str">
-        <v>11:42:09</v>
+        <v>11:42:20</v>
       </c>
       <c r="E63" t="str">
         <v>Manual</v>
@@ -1664,7 +1664,7 @@
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>200933</v>
+        <v>201825</v>
       </c>
       <c r="B64" t="str">
         <v>General Surgery</v>
@@ -1673,7 +1673,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D64" t="str">
-        <v>11:42:20</v>
+        <v>11:42:35</v>
       </c>
       <c r="E64" t="str">
         <v>Manual</v>
@@ -1684,7 +1684,7 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>201825</v>
+        <v>190801</v>
       </c>
       <c r="B65" t="str">
         <v>General Surgery</v>
@@ -1693,7 +1693,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D65" t="str">
-        <v>11:42:35</v>
+        <v>11:42:42</v>
       </c>
       <c r="E65" t="str">
         <v>Manual</v>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>190801</v>
+        <v>201465</v>
       </c>
       <c r="B66" t="str">
         <v>General Surgery</v>
@@ -1713,10 +1713,10 @@
         <v>11/10/2025</v>
       </c>
       <c r="D66" t="str">
-        <v>11:42:42</v>
+        <v>11:42:49</v>
       </c>
       <c r="E66" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F66" t="str">
         <v>dnasr281@gmail.com</v>
@@ -1724,7 +1724,7 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>201465</v>
+        <v>201171</v>
       </c>
       <c r="B67" t="str">
         <v>General Surgery</v>
@@ -1733,7 +1733,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D67" t="str">
-        <v>11:42:49</v>
+        <v>11:42:52</v>
       </c>
       <c r="E67" t="str">
         <v>Scan</v>
@@ -1744,7 +1744,7 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>201171</v>
+        <v>200491</v>
       </c>
       <c r="B68" t="str">
         <v>General Surgery</v>
@@ -1753,7 +1753,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D68" t="str">
-        <v>11:42:52</v>
+        <v>11:42:54</v>
       </c>
       <c r="E68" t="str">
         <v>Scan</v>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>200491</v>
+        <v>200490</v>
       </c>
       <c r="B69" t="str">
         <v>General Surgery</v>
@@ -1773,7 +1773,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D69" t="str">
-        <v>11:42:54</v>
+        <v>11:42:56</v>
       </c>
       <c r="E69" t="str">
         <v>Scan</v>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>200490</v>
+        <v>200228</v>
       </c>
       <c r="B70" t="str">
         <v>General Surgery</v>
@@ -1793,7 +1793,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D70" t="str">
-        <v>11:42:56</v>
+        <v>11:42:59</v>
       </c>
       <c r="E70" t="str">
         <v>Scan</v>
@@ -1804,7 +1804,7 @@
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>200228</v>
+        <v>201669</v>
       </c>
       <c r="B71" t="str">
         <v>General Surgery</v>
@@ -1813,7 +1813,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D71" t="str">
-        <v>11:42:59</v>
+        <v>11:43:01</v>
       </c>
       <c r="E71" t="str">
         <v>Scan</v>
@@ -1824,7 +1824,7 @@
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>201669</v>
+        <v>202004</v>
       </c>
       <c r="B72" t="str">
         <v>General Surgery</v>
@@ -1833,7 +1833,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D72" t="str">
-        <v>11:43:01</v>
+        <v>11:43:03</v>
       </c>
       <c r="E72" t="str">
         <v>Scan</v>
@@ -1844,7 +1844,7 @@
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>202004</v>
+        <v>200116</v>
       </c>
       <c r="B73" t="str">
         <v>General Surgery</v>
@@ -1853,7 +1853,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D73" t="str">
-        <v>11:43:03</v>
+        <v>11:43:05</v>
       </c>
       <c r="E73" t="str">
         <v>Scan</v>
@@ -1864,7 +1864,7 @@
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>200116</v>
+        <v>190796</v>
       </c>
       <c r="B74" t="str">
         <v>General Surgery</v>
@@ -1873,7 +1873,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D74" t="str">
-        <v>11:43:05</v>
+        <v>11:43:07</v>
       </c>
       <c r="E74" t="str">
         <v>Scan</v>
@@ -1884,7 +1884,7 @@
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>190796</v>
+        <v>190981</v>
       </c>
       <c r="B75" t="str">
         <v>General Surgery</v>
@@ -1893,7 +1893,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D75" t="str">
-        <v>11:43:07</v>
+        <v>11:43:09</v>
       </c>
       <c r="E75" t="str">
         <v>Scan</v>
@@ -1904,7 +1904,7 @@
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>190981</v>
+        <v>200163</v>
       </c>
       <c r="B76" t="str">
         <v>General Surgery</v>
@@ -1913,7 +1913,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D76" t="str">
-        <v>11:43:09</v>
+        <v>11:43:12</v>
       </c>
       <c r="E76" t="str">
         <v>Scan</v>
@@ -1924,7 +1924,7 @@
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>200163</v>
+        <v>191061</v>
       </c>
       <c r="B77" t="str">
         <v>General Surgery</v>
@@ -1933,7 +1933,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D77" t="str">
-        <v>11:43:12</v>
+        <v>11:43:15</v>
       </c>
       <c r="E77" t="str">
         <v>Scan</v>
@@ -1944,7 +1944,7 @@
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>191061</v>
+        <v>200744</v>
       </c>
       <c r="B78" t="str">
         <v>General Surgery</v>
@@ -1953,7 +1953,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D78" t="str">
-        <v>11:43:15</v>
+        <v>11:43:17</v>
       </c>
       <c r="E78" t="str">
         <v>Scan</v>
@@ -1964,7 +1964,7 @@
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>200744</v>
+        <v>201564</v>
       </c>
       <c r="B79" t="str">
         <v>General Surgery</v>
@@ -1973,7 +1973,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D79" t="str">
-        <v>11:43:17</v>
+        <v>11:43:20</v>
       </c>
       <c r="E79" t="str">
         <v>Scan</v>
@@ -1984,7 +1984,7 @@
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>201564</v>
+        <v>200804</v>
       </c>
       <c r="B80" t="str">
         <v>General Surgery</v>
@@ -1993,7 +1993,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D80" t="str">
-        <v>11:43:20</v>
+        <v>11:43:22</v>
       </c>
       <c r="E80" t="str">
         <v>Scan</v>
@@ -2004,7 +2004,7 @@
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>200804</v>
+        <v>200792</v>
       </c>
       <c r="B81" t="str">
         <v>General Surgery</v>
@@ -2013,7 +2013,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D81" t="str">
-        <v>11:43:22</v>
+        <v>11:43:24</v>
       </c>
       <c r="E81" t="str">
         <v>Scan</v>
@@ -2024,7 +2024,7 @@
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>200792</v>
+        <v>200628</v>
       </c>
       <c r="B82" t="str">
         <v>General Surgery</v>
@@ -2033,7 +2033,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D82" t="str">
-        <v>11:43:24</v>
+        <v>11:43:26</v>
       </c>
       <c r="E82" t="str">
         <v>Scan</v>
@@ -2044,7 +2044,7 @@
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>200628</v>
+        <v>211216</v>
       </c>
       <c r="B83" t="str">
         <v>General Surgery</v>
@@ -2053,7 +2053,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D83" t="str">
-        <v>11:43:26</v>
+        <v>11:43:28</v>
       </c>
       <c r="E83" t="str">
         <v>Scan</v>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>211216</v>
+        <v>211197</v>
       </c>
       <c r="B84" t="str">
         <v>General Surgery</v>
@@ -2073,7 +2073,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D84" t="str">
-        <v>11:43:28</v>
+        <v>11:43:31</v>
       </c>
       <c r="E84" t="str">
         <v>Scan</v>
@@ -2084,7 +2084,7 @@
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>211197</v>
+        <v>201397</v>
       </c>
       <c r="B85" t="str">
         <v>General Surgery</v>
@@ -2093,7 +2093,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D85" t="str">
-        <v>11:43:31</v>
+        <v>11:43:33</v>
       </c>
       <c r="E85" t="str">
         <v>Scan</v>
@@ -2104,7 +2104,7 @@
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>201397</v>
+        <v>200917</v>
       </c>
       <c r="B86" t="str">
         <v>General Surgery</v>
@@ -2113,7 +2113,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D86" t="str">
-        <v>11:43:33</v>
+        <v>11:43:35</v>
       </c>
       <c r="E86" t="str">
         <v>Scan</v>
@@ -2124,7 +2124,7 @@
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>200917</v>
+        <v>201051</v>
       </c>
       <c r="B87" t="str">
         <v>General Surgery</v>
@@ -2133,7 +2133,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D87" t="str">
-        <v>11:43:35</v>
+        <v>11:43:37</v>
       </c>
       <c r="E87" t="str">
         <v>Scan</v>
@@ -2144,7 +2144,7 @@
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>201051</v>
+        <v>201501</v>
       </c>
       <c r="B88" t="str">
         <v>General Surgery</v>
@@ -2153,7 +2153,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D88" t="str">
-        <v>11:43:37</v>
+        <v>11:43:40</v>
       </c>
       <c r="E88" t="str">
         <v>Scan</v>
@@ -2164,7 +2164,7 @@
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>201501</v>
+        <v>200905</v>
       </c>
       <c r="B89" t="str">
         <v>General Surgery</v>
@@ -2173,7 +2173,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D89" t="str">
-        <v>11:43:40</v>
+        <v>11:43:42</v>
       </c>
       <c r="E89" t="str">
         <v>Scan</v>
@@ -2184,7 +2184,7 @@
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>200905</v>
+        <v>200938</v>
       </c>
       <c r="B90" t="str">
         <v>General Surgery</v>
@@ -2193,7 +2193,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D90" t="str">
-        <v>11:43:42</v>
+        <v>11:43:45</v>
       </c>
       <c r="E90" t="str">
         <v>Scan</v>
@@ -2204,7 +2204,7 @@
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>200938</v>
+        <v>211043</v>
       </c>
       <c r="B91" t="str">
         <v>General Surgery</v>
@@ -2213,7 +2213,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D91" t="str">
-        <v>11:43:45</v>
+        <v>11:43:47</v>
       </c>
       <c r="E91" t="str">
         <v>Scan</v>
@@ -2224,7 +2224,7 @@
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>211043</v>
+        <v>211133</v>
       </c>
       <c r="B92" t="str">
         <v>General Surgery</v>
@@ -2233,7 +2233,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D92" t="str">
-        <v>11:43:47</v>
+        <v>11:43:49</v>
       </c>
       <c r="E92" t="str">
         <v>Scan</v>
@@ -2244,7 +2244,7 @@
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>211133</v>
+        <v>211741</v>
       </c>
       <c r="B93" t="str">
         <v>General Surgery</v>
@@ -2253,7 +2253,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D93" t="str">
-        <v>11:43:49</v>
+        <v>11:43:50</v>
       </c>
       <c r="E93" t="str">
         <v>Scan</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>211741</v>
+        <v>211245</v>
       </c>
       <c r="B94" t="str">
         <v>General Surgery</v>
@@ -2273,7 +2273,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D94" t="str">
-        <v>11:43:50</v>
+        <v>11:43:52</v>
       </c>
       <c r="E94" t="str">
         <v>Scan</v>
@@ -2284,7 +2284,7 @@
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>211245</v>
+        <v>190929</v>
       </c>
       <c r="B95" t="str">
         <v>General Surgery</v>
@@ -2293,7 +2293,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D95" t="str">
-        <v>11:43:52</v>
+        <v>11:43:55</v>
       </c>
       <c r="E95" t="str">
         <v>Scan</v>
@@ -2304,7 +2304,7 @@
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>190929</v>
+        <v>191119</v>
       </c>
       <c r="B96" t="str">
         <v>General Surgery</v>
@@ -2313,7 +2313,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D96" t="str">
-        <v>11:43:55</v>
+        <v>11:43:56</v>
       </c>
       <c r="E96" t="str">
         <v>Scan</v>
@@ -2324,7 +2324,7 @@
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>191119</v>
+        <v>211210</v>
       </c>
       <c r="B97" t="str">
         <v>General Surgery</v>
@@ -2333,10 +2333,10 @@
         <v>11/10/2025</v>
       </c>
       <c r="D97" t="str">
-        <v>11:43:56</v>
+        <v>11:44:43</v>
       </c>
       <c r="E97" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F97" t="str">
         <v>dnasr281@gmail.com</v>
@@ -2344,7 +2344,7 @@
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>211210</v>
+        <v>201880</v>
       </c>
       <c r="B98" t="str">
         <v>General Surgery</v>
@@ -2353,7 +2353,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D98" t="str">
-        <v>11:44:43</v>
+        <v>11:45:28</v>
       </c>
       <c r="E98" t="str">
         <v>Manual</v>
@@ -2364,7 +2364,7 @@
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>201880</v>
+        <v>211246</v>
       </c>
       <c r="B99" t="str">
         <v>General Surgery</v>
@@ -2373,7 +2373,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D99" t="str">
-        <v>11:45:28</v>
+        <v>11:45:59</v>
       </c>
       <c r="E99" t="str">
         <v>Manual</v>
@@ -2384,7 +2384,7 @@
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>211246</v>
+        <v>201823</v>
       </c>
       <c r="B100" t="str">
         <v>General Surgery</v>
@@ -2393,7 +2393,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D100" t="str">
-        <v>11:45:59</v>
+        <v>11:46:33</v>
       </c>
       <c r="E100" t="str">
         <v>Manual</v>
@@ -2404,7 +2404,7 @@
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>201823</v>
+        <v>200928</v>
       </c>
       <c r="B101" t="str">
         <v>General Surgery</v>
@@ -2413,7 +2413,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D101" t="str">
-        <v>11:46:33</v>
+        <v>11:47:11</v>
       </c>
       <c r="E101" t="str">
         <v>Manual</v>
@@ -2424,7 +2424,7 @@
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>200928</v>
+        <v>201237</v>
       </c>
       <c r="B102" t="str">
         <v>General Surgery</v>
@@ -2433,7 +2433,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D102" t="str">
-        <v>11:47:11</v>
+        <v>11:47:35</v>
       </c>
       <c r="E102" t="str">
         <v>Manual</v>
@@ -2444,7 +2444,7 @@
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>201237</v>
+        <v>201513</v>
       </c>
       <c r="B103" t="str">
         <v>General Surgery</v>
@@ -2453,7 +2453,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D103" t="str">
-        <v>11:47:35</v>
+        <v>11:48:02</v>
       </c>
       <c r="E103" t="str">
         <v>Manual</v>
@@ -2464,7 +2464,7 @@
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>201513</v>
+        <v>200997</v>
       </c>
       <c r="B104" t="str">
         <v>General Surgery</v>
@@ -2473,7 +2473,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D104" t="str">
-        <v>11:48:02</v>
+        <v>11:48:26</v>
       </c>
       <c r="E104" t="str">
         <v>Manual</v>
@@ -2484,7 +2484,7 @@
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>200997</v>
+        <v>181004</v>
       </c>
       <c r="B105" t="str">
         <v>General Surgery</v>
@@ -2493,7 +2493,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D105" t="str">
-        <v>11:48:26</v>
+        <v>11:48:49</v>
       </c>
       <c r="E105" t="str">
         <v>Manual</v>
@@ -2504,7 +2504,7 @@
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>181004</v>
+        <v>211121</v>
       </c>
       <c r="B106" t="str">
         <v>General Surgery</v>
@@ -2513,7 +2513,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D106" t="str">
-        <v>11:48:49</v>
+        <v>11:49:14</v>
       </c>
       <c r="E106" t="str">
         <v>Manual</v>
@@ -2524,7 +2524,7 @@
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>211121</v>
+        <v>201252</v>
       </c>
       <c r="B107" t="str">
         <v>General Surgery</v>
@@ -2533,7 +2533,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D107" t="str">
-        <v>11:49:14</v>
+        <v>11:49:29</v>
       </c>
       <c r="E107" t="str">
         <v>Manual</v>
@@ -2544,7 +2544,7 @@
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>201252</v>
+        <v>201023</v>
       </c>
       <c r="B108" t="str">
         <v>General Surgery</v>
@@ -2553,7 +2553,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D108" t="str">
-        <v>11:49:29</v>
+        <v>11:49:42</v>
       </c>
       <c r="E108" t="str">
         <v>Manual</v>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>201023</v>
+        <v>201253</v>
       </c>
       <c r="B109" t="str">
         <v>General Surgery</v>
@@ -2573,7 +2573,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D109" t="str">
-        <v>11:49:42</v>
+        <v>11:49:57</v>
       </c>
       <c r="E109" t="str">
         <v>Manual</v>
@@ -2584,7 +2584,7 @@
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>201253</v>
+        <v>201337</v>
       </c>
       <c r="B110" t="str">
         <v>General Surgery</v>
@@ -2593,7 +2593,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D110" t="str">
-        <v>11:49:57</v>
+        <v>11:50:11</v>
       </c>
       <c r="E110" t="str">
         <v>Manual</v>
@@ -2604,7 +2604,7 @@
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>201337</v>
+        <v>201572</v>
       </c>
       <c r="B111" t="str">
         <v>General Surgery</v>
@@ -2613,10 +2613,10 @@
         <v>11/10/2025</v>
       </c>
       <c r="D111" t="str">
-        <v>11:50:11</v>
+        <v>11:50:20</v>
       </c>
       <c r="E111" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F111" t="str">
         <v>dnasr281@gmail.com</v>
@@ -2624,7 +2624,7 @@
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>201572</v>
+        <v>201398</v>
       </c>
       <c r="B112" t="str">
         <v>General Surgery</v>
@@ -2633,38 +2633,18 @@
         <v>11/10/2025</v>
       </c>
       <c r="D112" t="str">
-        <v>11:50:20</v>
+        <v>11:50:41</v>
       </c>
       <c r="E112" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F112" t="str">
-        <v>dnasr281@gmail.com</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="str">
-        <v>201398</v>
-      </c>
-      <c r="B113" t="str">
-        <v>General Surgery</v>
-      </c>
-      <c r="C113" t="str">
-        <v>11/10/2025</v>
-      </c>
-      <c r="D113" t="str">
-        <v>11:50:41</v>
-      </c>
-      <c r="E113" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F113" t="str">
         <v>dnasr281@gmail.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F113"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F112"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Backup QR Scanner data - 2025-10-12T07:50:03.645Z - Cache Bust: 1760255403645
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_General_Surgery_scanner1760170816881_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
+++ b/log_history/Y4_B2526_General_Surgery_scanner1760170816881_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F112"/>
+  <dimension ref="A1:F111"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -804,7 +804,7 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>200742</v>
+        <v>201563</v>
       </c>
       <c r="B21" t="str">
         <v>General Surgery</v>
@@ -813,7 +813,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D21" t="str">
-        <v>11:27:56</v>
+        <v>11:28:13</v>
       </c>
       <c r="E21" t="str">
         <v>Manual</v>
@@ -824,7 +824,7 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>201563</v>
+        <v>180804</v>
       </c>
       <c r="B22" t="str">
         <v>General Surgery</v>
@@ -833,7 +833,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D22" t="str">
-        <v>11:28:13</v>
+        <v>11:28:23</v>
       </c>
       <c r="E22" t="str">
         <v>Manual</v>
@@ -844,7 +844,7 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>180804</v>
+        <v>211167</v>
       </c>
       <c r="B23" t="str">
         <v>General Surgery</v>
@@ -853,7 +853,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D23" t="str">
-        <v>11:28:23</v>
+        <v>11:28:31</v>
       </c>
       <c r="E23" t="str">
         <v>Manual</v>
@@ -864,7 +864,7 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>211167</v>
+        <v>211169</v>
       </c>
       <c r="B24" t="str">
         <v>General Surgery</v>
@@ -873,7 +873,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D24" t="str">
-        <v>11:28:31</v>
+        <v>11:28:41</v>
       </c>
       <c r="E24" t="str">
         <v>Manual</v>
@@ -884,7 +884,7 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>211169</v>
+        <v>211079</v>
       </c>
       <c r="B25" t="str">
         <v>General Surgery</v>
@@ -893,7 +893,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D25" t="str">
-        <v>11:28:41</v>
+        <v>11:28:48</v>
       </c>
       <c r="E25" t="str">
         <v>Manual</v>
@@ -904,7 +904,7 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>211079</v>
+        <v>200468</v>
       </c>
       <c r="B26" t="str">
         <v>General Surgery</v>
@@ -913,7 +913,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D26" t="str">
-        <v>11:28:48</v>
+        <v>11:29:01</v>
       </c>
       <c r="E26" t="str">
         <v>Manual</v>
@@ -924,7 +924,7 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>200468</v>
+        <v>191109</v>
       </c>
       <c r="B27" t="str">
         <v>General Surgery</v>
@@ -933,7 +933,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D27" t="str">
-        <v>11:29:01</v>
+        <v>11:29:08</v>
       </c>
       <c r="E27" t="str">
         <v>Manual</v>
@@ -944,7 +944,7 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>191109</v>
+        <v>191088</v>
       </c>
       <c r="B28" t="str">
         <v>General Surgery</v>
@@ -953,7 +953,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D28" t="str">
-        <v>11:29:08</v>
+        <v>11:29:17</v>
       </c>
       <c r="E28" t="str">
         <v>Manual</v>
@@ -964,7 +964,7 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>191088</v>
+        <v>200423</v>
       </c>
       <c r="B29" t="str">
         <v>General Surgery</v>
@@ -973,7 +973,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D29" t="str">
-        <v>11:29:17</v>
+        <v>11:29:25</v>
       </c>
       <c r="E29" t="str">
         <v>Manual</v>
@@ -984,7 +984,7 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>200423</v>
+        <v>190931</v>
       </c>
       <c r="B30" t="str">
         <v>General Surgery</v>
@@ -993,7 +993,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D30" t="str">
-        <v>11:29:25</v>
+        <v>11:29:35</v>
       </c>
       <c r="E30" t="str">
         <v>Manual</v>
@@ -1004,7 +1004,7 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>190931</v>
+        <v>190922</v>
       </c>
       <c r="B31" t="str">
         <v>General Surgery</v>
@@ -1013,7 +1013,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D31" t="str">
-        <v>11:29:35</v>
+        <v>11:29:50</v>
       </c>
       <c r="E31" t="str">
         <v>Manual</v>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>190922</v>
+        <v>191131</v>
       </c>
       <c r="B32" t="str">
         <v>General Surgery</v>
@@ -1033,7 +1033,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D32" t="str">
-        <v>11:29:50</v>
+        <v>11:30:02</v>
       </c>
       <c r="E32" t="str">
         <v>Manual</v>
@@ -1044,7 +1044,7 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>191131</v>
+        <v>190803</v>
       </c>
       <c r="B33" t="str">
         <v>General Surgery</v>
@@ -1053,7 +1053,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D33" t="str">
-        <v>11:30:02</v>
+        <v>11:30:15</v>
       </c>
       <c r="E33" t="str">
         <v>Manual</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>190803</v>
+        <v>181013</v>
       </c>
       <c r="B34" t="str">
         <v>General Surgery</v>
@@ -1073,7 +1073,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D34" t="str">
-        <v>11:30:15</v>
+        <v>11:30:22</v>
       </c>
       <c r="E34" t="str">
         <v>Manual</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>181013</v>
+        <v>201495</v>
       </c>
       <c r="B35" t="str">
         <v>General Surgery</v>
@@ -1093,7 +1093,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D35" t="str">
-        <v>11:30:22</v>
+        <v>11:30:50</v>
       </c>
       <c r="E35" t="str">
         <v>Manual</v>
@@ -1104,7 +1104,7 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>201495</v>
+        <v>201026</v>
       </c>
       <c r="B36" t="str">
         <v>General Surgery</v>
@@ -1113,7 +1113,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D36" t="str">
-        <v>11:30:50</v>
+        <v>11:33:15</v>
       </c>
       <c r="E36" t="str">
         <v>Manual</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>201026</v>
+        <v>200850</v>
       </c>
       <c r="B37" t="str">
         <v>General Surgery</v>
@@ -1133,7 +1133,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D37" t="str">
-        <v>11:33:15</v>
+        <v>11:33:26</v>
       </c>
       <c r="E37" t="str">
         <v>Manual</v>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>200850</v>
+        <v>200866</v>
       </c>
       <c r="B38" t="str">
         <v>General Surgery</v>
@@ -1153,7 +1153,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D38" t="str">
-        <v>11:33:26</v>
+        <v>11:33:36</v>
       </c>
       <c r="E38" t="str">
         <v>Manual</v>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>200866</v>
+        <v>211118</v>
       </c>
       <c r="B39" t="str">
         <v>General Surgery</v>
@@ -1173,7 +1173,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D39" t="str">
-        <v>11:33:36</v>
+        <v>11:36:25</v>
       </c>
       <c r="E39" t="str">
         <v>Manual</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>211118</v>
+        <v>200904</v>
       </c>
       <c r="B40" t="str">
         <v>General Surgery</v>
@@ -1193,7 +1193,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D40" t="str">
-        <v>11:36:25</v>
+        <v>11:37:01</v>
       </c>
       <c r="E40" t="str">
         <v>Manual</v>
@@ -1204,7 +1204,7 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>200904</v>
+        <v>201632</v>
       </c>
       <c r="B41" t="str">
         <v>General Surgery</v>
@@ -1213,7 +1213,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D41" t="str">
-        <v>11:37:01</v>
+        <v>11:37:08</v>
       </c>
       <c r="E41" t="str">
         <v>Manual</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>201632</v>
+        <v>201190</v>
       </c>
       <c r="B42" t="str">
         <v>General Surgery</v>
@@ -1233,7 +1233,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D42" t="str">
-        <v>11:37:08</v>
+        <v>11:37:15</v>
       </c>
       <c r="E42" t="str">
         <v>Manual</v>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>201190</v>
+        <v>200824</v>
       </c>
       <c r="B43" t="str">
         <v>General Surgery</v>
@@ -1253,7 +1253,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D43" t="str">
-        <v>11:37:15</v>
+        <v>11:37:21</v>
       </c>
       <c r="E43" t="str">
         <v>Manual</v>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>200824</v>
+        <v>201197</v>
       </c>
       <c r="B44" t="str">
         <v>General Surgery</v>
@@ -1273,7 +1273,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D44" t="str">
-        <v>11:37:21</v>
+        <v>11:37:28</v>
       </c>
       <c r="E44" t="str">
         <v>Manual</v>
@@ -1284,7 +1284,7 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>201197</v>
+        <v>200914</v>
       </c>
       <c r="B45" t="str">
         <v>General Surgery</v>
@@ -1293,7 +1293,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D45" t="str">
-        <v>11:37:28</v>
+        <v>11:37:39</v>
       </c>
       <c r="E45" t="str">
         <v>Manual</v>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>200914</v>
+        <v>201065</v>
       </c>
       <c r="B46" t="str">
         <v>General Surgery</v>
@@ -1313,7 +1313,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D46" t="str">
-        <v>11:37:39</v>
+        <v>11:38:11</v>
       </c>
       <c r="E46" t="str">
         <v>Manual</v>
@@ -1324,7 +1324,7 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>201065</v>
+        <v>191478</v>
       </c>
       <c r="B47" t="str">
         <v>General Surgery</v>
@@ -1333,7 +1333,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D47" t="str">
-        <v>11:38:11</v>
+        <v>11:38:32</v>
       </c>
       <c r="E47" t="str">
         <v>Manual</v>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>191478</v>
+        <v>200999</v>
       </c>
       <c r="B48" t="str">
         <v>General Surgery</v>
@@ -1353,7 +1353,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D48" t="str">
-        <v>11:38:32</v>
+        <v>11:38:40</v>
       </c>
       <c r="E48" t="str">
         <v>Manual</v>
@@ -1364,7 +1364,7 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>200999</v>
+        <v>201157</v>
       </c>
       <c r="B49" t="str">
         <v>General Surgery</v>
@@ -1373,7 +1373,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D49" t="str">
-        <v>11:38:40</v>
+        <v>11:38:51</v>
       </c>
       <c r="E49" t="str">
         <v>Manual</v>
@@ -1384,7 +1384,7 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>201157</v>
+        <v>190314</v>
       </c>
       <c r="B50" t="str">
         <v>General Surgery</v>
@@ -1393,7 +1393,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D50" t="str">
-        <v>11:38:51</v>
+        <v>11:39:02</v>
       </c>
       <c r="E50" t="str">
         <v>Manual</v>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>190314</v>
+        <v>202162</v>
       </c>
       <c r="B51" t="str">
         <v>General Surgery</v>
@@ -1413,7 +1413,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D51" t="str">
-        <v>11:39:02</v>
+        <v>11:39:12</v>
       </c>
       <c r="E51" t="str">
         <v>Manual</v>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>202162</v>
+        <v>201819</v>
       </c>
       <c r="B52" t="str">
         <v>General Surgery</v>
@@ -1433,7 +1433,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D52" t="str">
-        <v>11:39:12</v>
+        <v>11:39:21</v>
       </c>
       <c r="E52" t="str">
         <v>Manual</v>
@@ -1444,7 +1444,7 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>201819</v>
+        <v>201990</v>
       </c>
       <c r="B53" t="str">
         <v>General Surgery</v>
@@ -1453,7 +1453,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D53" t="str">
-        <v>11:39:21</v>
+        <v>11:39:29</v>
       </c>
       <c r="E53" t="str">
         <v>Manual</v>
@@ -1464,7 +1464,7 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>201990</v>
+        <v>211175</v>
       </c>
       <c r="B54" t="str">
         <v>General Surgery</v>
@@ -1473,7 +1473,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D54" t="str">
-        <v>11:39:29</v>
+        <v>11:39:42</v>
       </c>
       <c r="E54" t="str">
         <v>Manual</v>
@@ -1484,7 +1484,7 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>211175</v>
+        <v>201795</v>
       </c>
       <c r="B55" t="str">
         <v>General Surgery</v>
@@ -1493,7 +1493,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D55" t="str">
-        <v>11:39:42</v>
+        <v>11:39:58</v>
       </c>
       <c r="E55" t="str">
         <v>Manual</v>
@@ -1504,7 +1504,7 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>201795</v>
+        <v>211174</v>
       </c>
       <c r="B56" t="str">
         <v>General Surgery</v>
@@ -1513,7 +1513,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D56" t="str">
-        <v>11:39:58</v>
+        <v>11:41:21</v>
       </c>
       <c r="E56" t="str">
         <v>Manual</v>
@@ -1524,7 +1524,7 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>211174</v>
+        <v>211092</v>
       </c>
       <c r="B57" t="str">
         <v>General Surgery</v>
@@ -1533,7 +1533,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D57" t="str">
-        <v>11:41:21</v>
+        <v>11:41:29</v>
       </c>
       <c r="E57" t="str">
         <v>Manual</v>
@@ -1544,7 +1544,7 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>211092</v>
+        <v>211046</v>
       </c>
       <c r="B58" t="str">
         <v>General Surgery</v>
@@ -1553,7 +1553,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D58" t="str">
-        <v>11:41:29</v>
+        <v>11:41:38</v>
       </c>
       <c r="E58" t="str">
         <v>Manual</v>
@@ -1564,7 +1564,7 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>211046</v>
+        <v>211242</v>
       </c>
       <c r="B59" t="str">
         <v>General Surgery</v>
@@ -1573,7 +1573,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D59" t="str">
-        <v>11:41:38</v>
+        <v>11:41:50</v>
       </c>
       <c r="E59" t="str">
         <v>Manual</v>
@@ -1584,7 +1584,7 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>211242</v>
+        <v>211010</v>
       </c>
       <c r="B60" t="str">
         <v>General Surgery</v>
@@ -1593,7 +1593,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D60" t="str">
-        <v>11:41:50</v>
+        <v>11:41:58</v>
       </c>
       <c r="E60" t="str">
         <v>Manual</v>
@@ -1604,7 +1604,7 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>211010</v>
+        <v>190968</v>
       </c>
       <c r="B61" t="str">
         <v>General Surgery</v>
@@ -1613,7 +1613,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D61" t="str">
-        <v>11:41:58</v>
+        <v>11:42:09</v>
       </c>
       <c r="E61" t="str">
         <v>Manual</v>
@@ -1624,7 +1624,7 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>190968</v>
+        <v>200933</v>
       </c>
       <c r="B62" t="str">
         <v>General Surgery</v>
@@ -1633,7 +1633,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D62" t="str">
-        <v>11:42:09</v>
+        <v>11:42:20</v>
       </c>
       <c r="E62" t="str">
         <v>Manual</v>
@@ -1644,7 +1644,7 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>200933</v>
+        <v>201825</v>
       </c>
       <c r="B63" t="str">
         <v>General Surgery</v>
@@ -1653,7 +1653,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D63" t="str">
-        <v>11:42:20</v>
+        <v>11:42:35</v>
       </c>
       <c r="E63" t="str">
         <v>Manual</v>
@@ -1664,7 +1664,7 @@
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>201825</v>
+        <v>190801</v>
       </c>
       <c r="B64" t="str">
         <v>General Surgery</v>
@@ -1673,7 +1673,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D64" t="str">
-        <v>11:42:35</v>
+        <v>11:42:42</v>
       </c>
       <c r="E64" t="str">
         <v>Manual</v>
@@ -1684,7 +1684,7 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>190801</v>
+        <v>201465</v>
       </c>
       <c r="B65" t="str">
         <v>General Surgery</v>
@@ -1693,10 +1693,10 @@
         <v>11/10/2025</v>
       </c>
       <c r="D65" t="str">
-        <v>11:42:42</v>
+        <v>11:42:49</v>
       </c>
       <c r="E65" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F65" t="str">
         <v>dnasr281@gmail.com</v>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>201465</v>
+        <v>201171</v>
       </c>
       <c r="B66" t="str">
         <v>General Surgery</v>
@@ -1713,7 +1713,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D66" t="str">
-        <v>11:42:49</v>
+        <v>11:42:52</v>
       </c>
       <c r="E66" t="str">
         <v>Scan</v>
@@ -1724,7 +1724,7 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>201171</v>
+        <v>200491</v>
       </c>
       <c r="B67" t="str">
         <v>General Surgery</v>
@@ -1733,7 +1733,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D67" t="str">
-        <v>11:42:52</v>
+        <v>11:42:54</v>
       </c>
       <c r="E67" t="str">
         <v>Scan</v>
@@ -1744,7 +1744,7 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>200491</v>
+        <v>200490</v>
       </c>
       <c r="B68" t="str">
         <v>General Surgery</v>
@@ -1753,7 +1753,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D68" t="str">
-        <v>11:42:54</v>
+        <v>11:42:56</v>
       </c>
       <c r="E68" t="str">
         <v>Scan</v>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>200490</v>
+        <v>200228</v>
       </c>
       <c r="B69" t="str">
         <v>General Surgery</v>
@@ -1773,7 +1773,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D69" t="str">
-        <v>11:42:56</v>
+        <v>11:42:59</v>
       </c>
       <c r="E69" t="str">
         <v>Scan</v>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>200228</v>
+        <v>201669</v>
       </c>
       <c r="B70" t="str">
         <v>General Surgery</v>
@@ -1793,7 +1793,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D70" t="str">
-        <v>11:42:59</v>
+        <v>11:43:01</v>
       </c>
       <c r="E70" t="str">
         <v>Scan</v>
@@ -1804,7 +1804,7 @@
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>201669</v>
+        <v>202004</v>
       </c>
       <c r="B71" t="str">
         <v>General Surgery</v>
@@ -1813,7 +1813,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D71" t="str">
-        <v>11:43:01</v>
+        <v>11:43:03</v>
       </c>
       <c r="E71" t="str">
         <v>Scan</v>
@@ -1824,7 +1824,7 @@
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>202004</v>
+        <v>200116</v>
       </c>
       <c r="B72" t="str">
         <v>General Surgery</v>
@@ -1833,7 +1833,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D72" t="str">
-        <v>11:43:03</v>
+        <v>11:43:05</v>
       </c>
       <c r="E72" t="str">
         <v>Scan</v>
@@ -1844,7 +1844,7 @@
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>200116</v>
+        <v>190796</v>
       </c>
       <c r="B73" t="str">
         <v>General Surgery</v>
@@ -1853,7 +1853,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D73" t="str">
-        <v>11:43:05</v>
+        <v>11:43:07</v>
       </c>
       <c r="E73" t="str">
         <v>Scan</v>
@@ -1864,7 +1864,7 @@
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>190796</v>
+        <v>190981</v>
       </c>
       <c r="B74" t="str">
         <v>General Surgery</v>
@@ -1873,7 +1873,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D74" t="str">
-        <v>11:43:07</v>
+        <v>11:43:09</v>
       </c>
       <c r="E74" t="str">
         <v>Scan</v>
@@ -1884,7 +1884,7 @@
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>190981</v>
+        <v>200163</v>
       </c>
       <c r="B75" t="str">
         <v>General Surgery</v>
@@ -1893,7 +1893,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D75" t="str">
-        <v>11:43:09</v>
+        <v>11:43:12</v>
       </c>
       <c r="E75" t="str">
         <v>Scan</v>
@@ -1904,7 +1904,7 @@
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>200163</v>
+        <v>191061</v>
       </c>
       <c r="B76" t="str">
         <v>General Surgery</v>
@@ -1913,7 +1913,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D76" t="str">
-        <v>11:43:12</v>
+        <v>11:43:15</v>
       </c>
       <c r="E76" t="str">
         <v>Scan</v>
@@ -1924,7 +1924,7 @@
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>191061</v>
+        <v>200744</v>
       </c>
       <c r="B77" t="str">
         <v>General Surgery</v>
@@ -1933,7 +1933,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D77" t="str">
-        <v>11:43:15</v>
+        <v>11:43:17</v>
       </c>
       <c r="E77" t="str">
         <v>Scan</v>
@@ -1944,7 +1944,7 @@
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>200744</v>
+        <v>201564</v>
       </c>
       <c r="B78" t="str">
         <v>General Surgery</v>
@@ -1953,7 +1953,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D78" t="str">
-        <v>11:43:17</v>
+        <v>11:43:20</v>
       </c>
       <c r="E78" t="str">
         <v>Scan</v>
@@ -1964,7 +1964,7 @@
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>201564</v>
+        <v>200804</v>
       </c>
       <c r="B79" t="str">
         <v>General Surgery</v>
@@ -1973,7 +1973,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D79" t="str">
-        <v>11:43:20</v>
+        <v>11:43:22</v>
       </c>
       <c r="E79" t="str">
         <v>Scan</v>
@@ -1984,7 +1984,7 @@
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>200804</v>
+        <v>200792</v>
       </c>
       <c r="B80" t="str">
         <v>General Surgery</v>
@@ -1993,7 +1993,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D80" t="str">
-        <v>11:43:22</v>
+        <v>11:43:24</v>
       </c>
       <c r="E80" t="str">
         <v>Scan</v>
@@ -2004,7 +2004,7 @@
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>200792</v>
+        <v>200628</v>
       </c>
       <c r="B81" t="str">
         <v>General Surgery</v>
@@ -2013,7 +2013,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D81" t="str">
-        <v>11:43:24</v>
+        <v>11:43:26</v>
       </c>
       <c r="E81" t="str">
         <v>Scan</v>
@@ -2024,7 +2024,7 @@
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>200628</v>
+        <v>211216</v>
       </c>
       <c r="B82" t="str">
         <v>General Surgery</v>
@@ -2033,7 +2033,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D82" t="str">
-        <v>11:43:26</v>
+        <v>11:43:28</v>
       </c>
       <c r="E82" t="str">
         <v>Scan</v>
@@ -2044,7 +2044,7 @@
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>211216</v>
+        <v>211197</v>
       </c>
       <c r="B83" t="str">
         <v>General Surgery</v>
@@ -2053,7 +2053,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D83" t="str">
-        <v>11:43:28</v>
+        <v>11:43:31</v>
       </c>
       <c r="E83" t="str">
         <v>Scan</v>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>211197</v>
+        <v>201397</v>
       </c>
       <c r="B84" t="str">
         <v>General Surgery</v>
@@ -2073,7 +2073,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D84" t="str">
-        <v>11:43:31</v>
+        <v>11:43:33</v>
       </c>
       <c r="E84" t="str">
         <v>Scan</v>
@@ -2084,7 +2084,7 @@
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>201397</v>
+        <v>200917</v>
       </c>
       <c r="B85" t="str">
         <v>General Surgery</v>
@@ -2093,7 +2093,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D85" t="str">
-        <v>11:43:33</v>
+        <v>11:43:35</v>
       </c>
       <c r="E85" t="str">
         <v>Scan</v>
@@ -2104,7 +2104,7 @@
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>200917</v>
+        <v>201051</v>
       </c>
       <c r="B86" t="str">
         <v>General Surgery</v>
@@ -2113,7 +2113,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D86" t="str">
-        <v>11:43:35</v>
+        <v>11:43:37</v>
       </c>
       <c r="E86" t="str">
         <v>Scan</v>
@@ -2124,7 +2124,7 @@
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>201051</v>
+        <v>201501</v>
       </c>
       <c r="B87" t="str">
         <v>General Surgery</v>
@@ -2133,7 +2133,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D87" t="str">
-        <v>11:43:37</v>
+        <v>11:43:40</v>
       </c>
       <c r="E87" t="str">
         <v>Scan</v>
@@ -2144,7 +2144,7 @@
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>201501</v>
+        <v>200905</v>
       </c>
       <c r="B88" t="str">
         <v>General Surgery</v>
@@ -2153,7 +2153,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D88" t="str">
-        <v>11:43:40</v>
+        <v>11:43:42</v>
       </c>
       <c r="E88" t="str">
         <v>Scan</v>
@@ -2164,7 +2164,7 @@
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>200905</v>
+        <v>200938</v>
       </c>
       <c r="B89" t="str">
         <v>General Surgery</v>
@@ -2173,7 +2173,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D89" t="str">
-        <v>11:43:42</v>
+        <v>11:43:45</v>
       </c>
       <c r="E89" t="str">
         <v>Scan</v>
@@ -2184,7 +2184,7 @@
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>200938</v>
+        <v>211043</v>
       </c>
       <c r="B90" t="str">
         <v>General Surgery</v>
@@ -2193,7 +2193,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D90" t="str">
-        <v>11:43:45</v>
+        <v>11:43:47</v>
       </c>
       <c r="E90" t="str">
         <v>Scan</v>
@@ -2204,7 +2204,7 @@
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>211043</v>
+        <v>211133</v>
       </c>
       <c r="B91" t="str">
         <v>General Surgery</v>
@@ -2213,7 +2213,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D91" t="str">
-        <v>11:43:47</v>
+        <v>11:43:49</v>
       </c>
       <c r="E91" t="str">
         <v>Scan</v>
@@ -2224,7 +2224,7 @@
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>211133</v>
+        <v>211741</v>
       </c>
       <c r="B92" t="str">
         <v>General Surgery</v>
@@ -2233,7 +2233,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D92" t="str">
-        <v>11:43:49</v>
+        <v>11:43:50</v>
       </c>
       <c r="E92" t="str">
         <v>Scan</v>
@@ -2244,7 +2244,7 @@
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>211741</v>
+        <v>211245</v>
       </c>
       <c r="B93" t="str">
         <v>General Surgery</v>
@@ -2253,7 +2253,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D93" t="str">
-        <v>11:43:50</v>
+        <v>11:43:52</v>
       </c>
       <c r="E93" t="str">
         <v>Scan</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>211245</v>
+        <v>190929</v>
       </c>
       <c r="B94" t="str">
         <v>General Surgery</v>
@@ -2273,7 +2273,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D94" t="str">
-        <v>11:43:52</v>
+        <v>11:43:55</v>
       </c>
       <c r="E94" t="str">
         <v>Scan</v>
@@ -2284,7 +2284,7 @@
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>190929</v>
+        <v>191119</v>
       </c>
       <c r="B95" t="str">
         <v>General Surgery</v>
@@ -2293,7 +2293,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D95" t="str">
-        <v>11:43:55</v>
+        <v>11:43:56</v>
       </c>
       <c r="E95" t="str">
         <v>Scan</v>
@@ -2304,7 +2304,7 @@
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>191119</v>
+        <v>211210</v>
       </c>
       <c r="B96" t="str">
         <v>General Surgery</v>
@@ -2313,10 +2313,10 @@
         <v>11/10/2025</v>
       </c>
       <c r="D96" t="str">
-        <v>11:43:56</v>
+        <v>11:44:43</v>
       </c>
       <c r="E96" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F96" t="str">
         <v>dnasr281@gmail.com</v>
@@ -2324,7 +2324,7 @@
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>211210</v>
+        <v>201880</v>
       </c>
       <c r="B97" t="str">
         <v>General Surgery</v>
@@ -2333,7 +2333,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D97" t="str">
-        <v>11:44:43</v>
+        <v>11:45:28</v>
       </c>
       <c r="E97" t="str">
         <v>Manual</v>
@@ -2344,7 +2344,7 @@
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>201880</v>
+        <v>211246</v>
       </c>
       <c r="B98" t="str">
         <v>General Surgery</v>
@@ -2353,7 +2353,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D98" t="str">
-        <v>11:45:28</v>
+        <v>11:45:59</v>
       </c>
       <c r="E98" t="str">
         <v>Manual</v>
@@ -2364,7 +2364,7 @@
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>211246</v>
+        <v>201823</v>
       </c>
       <c r="B99" t="str">
         <v>General Surgery</v>
@@ -2373,7 +2373,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D99" t="str">
-        <v>11:45:59</v>
+        <v>11:46:33</v>
       </c>
       <c r="E99" t="str">
         <v>Manual</v>
@@ -2384,7 +2384,7 @@
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>201823</v>
+        <v>200928</v>
       </c>
       <c r="B100" t="str">
         <v>General Surgery</v>
@@ -2393,7 +2393,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D100" t="str">
-        <v>11:46:33</v>
+        <v>11:47:11</v>
       </c>
       <c r="E100" t="str">
         <v>Manual</v>
@@ -2404,7 +2404,7 @@
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>200928</v>
+        <v>201237</v>
       </c>
       <c r="B101" t="str">
         <v>General Surgery</v>
@@ -2413,7 +2413,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D101" t="str">
-        <v>11:47:11</v>
+        <v>11:47:35</v>
       </c>
       <c r="E101" t="str">
         <v>Manual</v>
@@ -2424,7 +2424,7 @@
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>201237</v>
+        <v>201513</v>
       </c>
       <c r="B102" t="str">
         <v>General Surgery</v>
@@ -2433,7 +2433,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D102" t="str">
-        <v>11:47:35</v>
+        <v>11:48:02</v>
       </c>
       <c r="E102" t="str">
         <v>Manual</v>
@@ -2444,7 +2444,7 @@
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>201513</v>
+        <v>200997</v>
       </c>
       <c r="B103" t="str">
         <v>General Surgery</v>
@@ -2453,7 +2453,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D103" t="str">
-        <v>11:48:02</v>
+        <v>11:48:26</v>
       </c>
       <c r="E103" t="str">
         <v>Manual</v>
@@ -2464,7 +2464,7 @@
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>200997</v>
+        <v>181004</v>
       </c>
       <c r="B104" t="str">
         <v>General Surgery</v>
@@ -2473,7 +2473,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D104" t="str">
-        <v>11:48:26</v>
+        <v>11:48:49</v>
       </c>
       <c r="E104" t="str">
         <v>Manual</v>
@@ -2484,7 +2484,7 @@
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>181004</v>
+        <v>211121</v>
       </c>
       <c r="B105" t="str">
         <v>General Surgery</v>
@@ -2493,7 +2493,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D105" t="str">
-        <v>11:48:49</v>
+        <v>11:49:14</v>
       </c>
       <c r="E105" t="str">
         <v>Manual</v>
@@ -2504,7 +2504,7 @@
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>211121</v>
+        <v>201252</v>
       </c>
       <c r="B106" t="str">
         <v>General Surgery</v>
@@ -2513,7 +2513,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D106" t="str">
-        <v>11:49:14</v>
+        <v>11:49:29</v>
       </c>
       <c r="E106" t="str">
         <v>Manual</v>
@@ -2524,7 +2524,7 @@
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>201252</v>
+        <v>201023</v>
       </c>
       <c r="B107" t="str">
         <v>General Surgery</v>
@@ -2533,7 +2533,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D107" t="str">
-        <v>11:49:29</v>
+        <v>11:49:42</v>
       </c>
       <c r="E107" t="str">
         <v>Manual</v>
@@ -2544,7 +2544,7 @@
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>201023</v>
+        <v>201253</v>
       </c>
       <c r="B108" t="str">
         <v>General Surgery</v>
@@ -2553,7 +2553,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D108" t="str">
-        <v>11:49:42</v>
+        <v>11:49:57</v>
       </c>
       <c r="E108" t="str">
         <v>Manual</v>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>201253</v>
+        <v>201337</v>
       </c>
       <c r="B109" t="str">
         <v>General Surgery</v>
@@ -2573,7 +2573,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D109" t="str">
-        <v>11:49:57</v>
+        <v>11:50:11</v>
       </c>
       <c r="E109" t="str">
         <v>Manual</v>
@@ -2584,7 +2584,7 @@
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>201337</v>
+        <v>201572</v>
       </c>
       <c r="B110" t="str">
         <v>General Surgery</v>
@@ -2593,10 +2593,10 @@
         <v>11/10/2025</v>
       </c>
       <c r="D110" t="str">
-        <v>11:50:11</v>
+        <v>11:50:20</v>
       </c>
       <c r="E110" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F110" t="str">
         <v>dnasr281@gmail.com</v>
@@ -2604,7 +2604,7 @@
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>201572</v>
+        <v>201398</v>
       </c>
       <c r="B111" t="str">
         <v>General Surgery</v>
@@ -2613,38 +2613,18 @@
         <v>11/10/2025</v>
       </c>
       <c r="D111" t="str">
-        <v>11:50:20</v>
+        <v>11:50:41</v>
       </c>
       <c r="E111" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F111" t="str">
-        <v>dnasr281@gmail.com</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="str">
-        <v>201398</v>
-      </c>
-      <c r="B112" t="str">
-        <v>General Surgery</v>
-      </c>
-      <c r="C112" t="str">
-        <v>11/10/2025</v>
-      </c>
-      <c r="D112" t="str">
-        <v>11:50:41</v>
-      </c>
-      <c r="E112" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F112" t="str">
         <v>dnasr281@gmail.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F112"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F111"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update edited session - 2025-10-12T07:53:19.683Z - Cache Bust ID: 1760255599683ugcl2h7sw
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_General_Surgery_scanner1760170816881_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
+++ b/log_history/Y4_B2526_General_Surgery_scanner1760170816881_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="General_Surgery" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F111"/>
+  <dimension ref="A1:F110"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -784,7 +784,7 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>191258</v>
+        <v>201563</v>
       </c>
       <c r="B20" t="str">
         <v>General Surgery</v>
@@ -793,7 +793,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D20" t="str">
-        <v>11:27:36</v>
+        <v>11:28:13</v>
       </c>
       <c r="E20" t="str">
         <v>Manual</v>
@@ -804,7 +804,7 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>201563</v>
+        <v>180804</v>
       </c>
       <c r="B21" t="str">
         <v>General Surgery</v>
@@ -813,7 +813,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D21" t="str">
-        <v>11:28:13</v>
+        <v>11:28:23</v>
       </c>
       <c r="E21" t="str">
         <v>Manual</v>
@@ -824,7 +824,7 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>180804</v>
+        <v>211167</v>
       </c>
       <c r="B22" t="str">
         <v>General Surgery</v>
@@ -833,7 +833,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D22" t="str">
-        <v>11:28:23</v>
+        <v>11:28:31</v>
       </c>
       <c r="E22" t="str">
         <v>Manual</v>
@@ -844,7 +844,7 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>211167</v>
+        <v>211169</v>
       </c>
       <c r="B23" t="str">
         <v>General Surgery</v>
@@ -853,7 +853,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D23" t="str">
-        <v>11:28:31</v>
+        <v>11:28:41</v>
       </c>
       <c r="E23" t="str">
         <v>Manual</v>
@@ -864,7 +864,7 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>211169</v>
+        <v>211079</v>
       </c>
       <c r="B24" t="str">
         <v>General Surgery</v>
@@ -873,7 +873,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D24" t="str">
-        <v>11:28:41</v>
+        <v>11:28:48</v>
       </c>
       <c r="E24" t="str">
         <v>Manual</v>
@@ -884,7 +884,7 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>211079</v>
+        <v>200468</v>
       </c>
       <c r="B25" t="str">
         <v>General Surgery</v>
@@ -893,7 +893,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D25" t="str">
-        <v>11:28:48</v>
+        <v>11:29:01</v>
       </c>
       <c r="E25" t="str">
         <v>Manual</v>
@@ -904,7 +904,7 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>200468</v>
+        <v>191109</v>
       </c>
       <c r="B26" t="str">
         <v>General Surgery</v>
@@ -913,7 +913,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D26" t="str">
-        <v>11:29:01</v>
+        <v>11:29:08</v>
       </c>
       <c r="E26" t="str">
         <v>Manual</v>
@@ -924,7 +924,7 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>191109</v>
+        <v>191088</v>
       </c>
       <c r="B27" t="str">
         <v>General Surgery</v>
@@ -933,7 +933,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D27" t="str">
-        <v>11:29:08</v>
+        <v>11:29:17</v>
       </c>
       <c r="E27" t="str">
         <v>Manual</v>
@@ -944,7 +944,7 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>191088</v>
+        <v>200423</v>
       </c>
       <c r="B28" t="str">
         <v>General Surgery</v>
@@ -953,7 +953,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D28" t="str">
-        <v>11:29:17</v>
+        <v>11:29:25</v>
       </c>
       <c r="E28" t="str">
         <v>Manual</v>
@@ -964,7 +964,7 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>200423</v>
+        <v>190931</v>
       </c>
       <c r="B29" t="str">
         <v>General Surgery</v>
@@ -973,7 +973,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D29" t="str">
-        <v>11:29:25</v>
+        <v>11:29:35</v>
       </c>
       <c r="E29" t="str">
         <v>Manual</v>
@@ -984,7 +984,7 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>190931</v>
+        <v>190922</v>
       </c>
       <c r="B30" t="str">
         <v>General Surgery</v>
@@ -993,7 +993,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D30" t="str">
-        <v>11:29:35</v>
+        <v>11:29:50</v>
       </c>
       <c r="E30" t="str">
         <v>Manual</v>
@@ -1004,7 +1004,7 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>190922</v>
+        <v>191131</v>
       </c>
       <c r="B31" t="str">
         <v>General Surgery</v>
@@ -1013,7 +1013,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D31" t="str">
-        <v>11:29:50</v>
+        <v>11:30:02</v>
       </c>
       <c r="E31" t="str">
         <v>Manual</v>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>191131</v>
+        <v>190803</v>
       </c>
       <c r="B32" t="str">
         <v>General Surgery</v>
@@ -1033,7 +1033,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D32" t="str">
-        <v>11:30:02</v>
+        <v>11:30:15</v>
       </c>
       <c r="E32" t="str">
         <v>Manual</v>
@@ -1044,7 +1044,7 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>190803</v>
+        <v>181013</v>
       </c>
       <c r="B33" t="str">
         <v>General Surgery</v>
@@ -1053,7 +1053,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D33" t="str">
-        <v>11:30:15</v>
+        <v>11:30:22</v>
       </c>
       <c r="E33" t="str">
         <v>Manual</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>181013</v>
+        <v>201495</v>
       </c>
       <c r="B34" t="str">
         <v>General Surgery</v>
@@ -1073,7 +1073,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D34" t="str">
-        <v>11:30:22</v>
+        <v>11:30:50</v>
       </c>
       <c r="E34" t="str">
         <v>Manual</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>201495</v>
+        <v>201026</v>
       </c>
       <c r="B35" t="str">
         <v>General Surgery</v>
@@ -1093,7 +1093,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D35" t="str">
-        <v>11:30:50</v>
+        <v>11:33:15</v>
       </c>
       <c r="E35" t="str">
         <v>Manual</v>
@@ -1104,7 +1104,7 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>201026</v>
+        <v>200850</v>
       </c>
       <c r="B36" t="str">
         <v>General Surgery</v>
@@ -1113,7 +1113,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D36" t="str">
-        <v>11:33:15</v>
+        <v>11:33:26</v>
       </c>
       <c r="E36" t="str">
         <v>Manual</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>200850</v>
+        <v>200866</v>
       </c>
       <c r="B37" t="str">
         <v>General Surgery</v>
@@ -1133,7 +1133,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D37" t="str">
-        <v>11:33:26</v>
+        <v>11:33:36</v>
       </c>
       <c r="E37" t="str">
         <v>Manual</v>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>200866</v>
+        <v>211118</v>
       </c>
       <c r="B38" t="str">
         <v>General Surgery</v>
@@ -1153,7 +1153,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D38" t="str">
-        <v>11:33:36</v>
+        <v>11:36:25</v>
       </c>
       <c r="E38" t="str">
         <v>Manual</v>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>211118</v>
+        <v>200904</v>
       </c>
       <c r="B39" t="str">
         <v>General Surgery</v>
@@ -1173,7 +1173,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D39" t="str">
-        <v>11:36:25</v>
+        <v>11:37:01</v>
       </c>
       <c r="E39" t="str">
         <v>Manual</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>200904</v>
+        <v>201632</v>
       </c>
       <c r="B40" t="str">
         <v>General Surgery</v>
@@ -1193,7 +1193,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D40" t="str">
-        <v>11:37:01</v>
+        <v>11:37:08</v>
       </c>
       <c r="E40" t="str">
         <v>Manual</v>
@@ -1204,7 +1204,7 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>201632</v>
+        <v>201190</v>
       </c>
       <c r="B41" t="str">
         <v>General Surgery</v>
@@ -1213,7 +1213,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D41" t="str">
-        <v>11:37:08</v>
+        <v>11:37:15</v>
       </c>
       <c r="E41" t="str">
         <v>Manual</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>201190</v>
+        <v>200824</v>
       </c>
       <c r="B42" t="str">
         <v>General Surgery</v>
@@ -1233,7 +1233,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D42" t="str">
-        <v>11:37:15</v>
+        <v>11:37:21</v>
       </c>
       <c r="E42" t="str">
         <v>Manual</v>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>200824</v>
+        <v>201197</v>
       </c>
       <c r="B43" t="str">
         <v>General Surgery</v>
@@ -1253,7 +1253,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D43" t="str">
-        <v>11:37:21</v>
+        <v>11:37:28</v>
       </c>
       <c r="E43" t="str">
         <v>Manual</v>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>201197</v>
+        <v>200914</v>
       </c>
       <c r="B44" t="str">
         <v>General Surgery</v>
@@ -1273,7 +1273,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D44" t="str">
-        <v>11:37:28</v>
+        <v>11:37:39</v>
       </c>
       <c r="E44" t="str">
         <v>Manual</v>
@@ -1284,7 +1284,7 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>200914</v>
+        <v>201065</v>
       </c>
       <c r="B45" t="str">
         <v>General Surgery</v>
@@ -1293,7 +1293,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D45" t="str">
-        <v>11:37:39</v>
+        <v>11:38:11</v>
       </c>
       <c r="E45" t="str">
         <v>Manual</v>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>201065</v>
+        <v>191478</v>
       </c>
       <c r="B46" t="str">
         <v>General Surgery</v>
@@ -1313,7 +1313,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D46" t="str">
-        <v>11:38:11</v>
+        <v>11:38:32</v>
       </c>
       <c r="E46" t="str">
         <v>Manual</v>
@@ -1324,7 +1324,7 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>191478</v>
+        <v>200999</v>
       </c>
       <c r="B47" t="str">
         <v>General Surgery</v>
@@ -1333,7 +1333,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D47" t="str">
-        <v>11:38:32</v>
+        <v>11:38:40</v>
       </c>
       <c r="E47" t="str">
         <v>Manual</v>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>200999</v>
+        <v>201157</v>
       </c>
       <c r="B48" t="str">
         <v>General Surgery</v>
@@ -1353,7 +1353,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D48" t="str">
-        <v>11:38:40</v>
+        <v>11:38:51</v>
       </c>
       <c r="E48" t="str">
         <v>Manual</v>
@@ -1364,7 +1364,7 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>201157</v>
+        <v>190314</v>
       </c>
       <c r="B49" t="str">
         <v>General Surgery</v>
@@ -1373,7 +1373,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D49" t="str">
-        <v>11:38:51</v>
+        <v>11:39:02</v>
       </c>
       <c r="E49" t="str">
         <v>Manual</v>
@@ -1384,7 +1384,7 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>190314</v>
+        <v>202162</v>
       </c>
       <c r="B50" t="str">
         <v>General Surgery</v>
@@ -1393,7 +1393,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D50" t="str">
-        <v>11:39:02</v>
+        <v>11:39:12</v>
       </c>
       <c r="E50" t="str">
         <v>Manual</v>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>202162</v>
+        <v>201819</v>
       </c>
       <c r="B51" t="str">
         <v>General Surgery</v>
@@ -1413,7 +1413,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D51" t="str">
-        <v>11:39:12</v>
+        <v>11:39:21</v>
       </c>
       <c r="E51" t="str">
         <v>Manual</v>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>201819</v>
+        <v>201990</v>
       </c>
       <c r="B52" t="str">
         <v>General Surgery</v>
@@ -1433,7 +1433,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D52" t="str">
-        <v>11:39:21</v>
+        <v>11:39:29</v>
       </c>
       <c r="E52" t="str">
         <v>Manual</v>
@@ -1444,7 +1444,7 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>201990</v>
+        <v>211175</v>
       </c>
       <c r="B53" t="str">
         <v>General Surgery</v>
@@ -1453,7 +1453,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D53" t="str">
-        <v>11:39:29</v>
+        <v>11:39:42</v>
       </c>
       <c r="E53" t="str">
         <v>Manual</v>
@@ -1464,7 +1464,7 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>211175</v>
+        <v>201795</v>
       </c>
       <c r="B54" t="str">
         <v>General Surgery</v>
@@ -1473,7 +1473,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D54" t="str">
-        <v>11:39:42</v>
+        <v>11:39:58</v>
       </c>
       <c r="E54" t="str">
         <v>Manual</v>
@@ -1484,7 +1484,7 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>201795</v>
+        <v>211174</v>
       </c>
       <c r="B55" t="str">
         <v>General Surgery</v>
@@ -1493,7 +1493,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D55" t="str">
-        <v>11:39:58</v>
+        <v>11:41:21</v>
       </c>
       <c r="E55" t="str">
         <v>Manual</v>
@@ -1504,7 +1504,7 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>211174</v>
+        <v>211092</v>
       </c>
       <c r="B56" t="str">
         <v>General Surgery</v>
@@ -1513,7 +1513,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D56" t="str">
-        <v>11:41:21</v>
+        <v>11:41:29</v>
       </c>
       <c r="E56" t="str">
         <v>Manual</v>
@@ -1524,7 +1524,7 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>211092</v>
+        <v>211046</v>
       </c>
       <c r="B57" t="str">
         <v>General Surgery</v>
@@ -1533,7 +1533,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D57" t="str">
-        <v>11:41:29</v>
+        <v>11:41:38</v>
       </c>
       <c r="E57" t="str">
         <v>Manual</v>
@@ -1544,7 +1544,7 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>211046</v>
+        <v>211242</v>
       </c>
       <c r="B58" t="str">
         <v>General Surgery</v>
@@ -1553,7 +1553,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D58" t="str">
-        <v>11:41:38</v>
+        <v>11:41:50</v>
       </c>
       <c r="E58" t="str">
         <v>Manual</v>
@@ -1564,7 +1564,7 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>211242</v>
+        <v>211010</v>
       </c>
       <c r="B59" t="str">
         <v>General Surgery</v>
@@ -1573,7 +1573,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D59" t="str">
-        <v>11:41:50</v>
+        <v>11:41:58</v>
       </c>
       <c r="E59" t="str">
         <v>Manual</v>
@@ -1584,7 +1584,7 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>211010</v>
+        <v>190968</v>
       </c>
       <c r="B60" t="str">
         <v>General Surgery</v>
@@ -1593,7 +1593,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D60" t="str">
-        <v>11:41:58</v>
+        <v>11:42:09</v>
       </c>
       <c r="E60" t="str">
         <v>Manual</v>
@@ -1604,7 +1604,7 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>190968</v>
+        <v>200933</v>
       </c>
       <c r="B61" t="str">
         <v>General Surgery</v>
@@ -1613,7 +1613,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D61" t="str">
-        <v>11:42:09</v>
+        <v>11:42:20</v>
       </c>
       <c r="E61" t="str">
         <v>Manual</v>
@@ -1624,7 +1624,7 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>200933</v>
+        <v>201825</v>
       </c>
       <c r="B62" t="str">
         <v>General Surgery</v>
@@ -1633,7 +1633,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D62" t="str">
-        <v>11:42:20</v>
+        <v>11:42:35</v>
       </c>
       <c r="E62" t="str">
         <v>Manual</v>
@@ -1644,7 +1644,7 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>201825</v>
+        <v>190801</v>
       </c>
       <c r="B63" t="str">
         <v>General Surgery</v>
@@ -1653,7 +1653,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D63" t="str">
-        <v>11:42:35</v>
+        <v>11:42:42</v>
       </c>
       <c r="E63" t="str">
         <v>Manual</v>
@@ -1664,7 +1664,7 @@
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>190801</v>
+        <v>201465</v>
       </c>
       <c r="B64" t="str">
         <v>General Surgery</v>
@@ -1673,10 +1673,10 @@
         <v>11/10/2025</v>
       </c>
       <c r="D64" t="str">
-        <v>11:42:42</v>
+        <v>11:42:49</v>
       </c>
       <c r="E64" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F64" t="str">
         <v>dnasr281@gmail.com</v>
@@ -1684,7 +1684,7 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>201465</v>
+        <v>201171</v>
       </c>
       <c r="B65" t="str">
         <v>General Surgery</v>
@@ -1693,7 +1693,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D65" t="str">
-        <v>11:42:49</v>
+        <v>11:42:52</v>
       </c>
       <c r="E65" t="str">
         <v>Scan</v>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>201171</v>
+        <v>200491</v>
       </c>
       <c r="B66" t="str">
         <v>General Surgery</v>
@@ -1713,7 +1713,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D66" t="str">
-        <v>11:42:52</v>
+        <v>11:42:54</v>
       </c>
       <c r="E66" t="str">
         <v>Scan</v>
@@ -1724,7 +1724,7 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>200491</v>
+        <v>200490</v>
       </c>
       <c r="B67" t="str">
         <v>General Surgery</v>
@@ -1733,7 +1733,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D67" t="str">
-        <v>11:42:54</v>
+        <v>11:42:56</v>
       </c>
       <c r="E67" t="str">
         <v>Scan</v>
@@ -1744,7 +1744,7 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>200490</v>
+        <v>200228</v>
       </c>
       <c r="B68" t="str">
         <v>General Surgery</v>
@@ -1753,7 +1753,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D68" t="str">
-        <v>11:42:56</v>
+        <v>11:42:59</v>
       </c>
       <c r="E68" t="str">
         <v>Scan</v>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>200228</v>
+        <v>201669</v>
       </c>
       <c r="B69" t="str">
         <v>General Surgery</v>
@@ -1773,7 +1773,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D69" t="str">
-        <v>11:42:59</v>
+        <v>11:43:01</v>
       </c>
       <c r="E69" t="str">
         <v>Scan</v>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>201669</v>
+        <v>202004</v>
       </c>
       <c r="B70" t="str">
         <v>General Surgery</v>
@@ -1793,7 +1793,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D70" t="str">
-        <v>11:43:01</v>
+        <v>11:43:03</v>
       </c>
       <c r="E70" t="str">
         <v>Scan</v>
@@ -1804,7 +1804,7 @@
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>202004</v>
+        <v>200116</v>
       </c>
       <c r="B71" t="str">
         <v>General Surgery</v>
@@ -1813,7 +1813,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D71" t="str">
-        <v>11:43:03</v>
+        <v>11:43:05</v>
       </c>
       <c r="E71" t="str">
         <v>Scan</v>
@@ -1824,7 +1824,7 @@
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>200116</v>
+        <v>190796</v>
       </c>
       <c r="B72" t="str">
         <v>General Surgery</v>
@@ -1833,7 +1833,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D72" t="str">
-        <v>11:43:05</v>
+        <v>11:43:07</v>
       </c>
       <c r="E72" t="str">
         <v>Scan</v>
@@ -1844,7 +1844,7 @@
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>190796</v>
+        <v>190981</v>
       </c>
       <c r="B73" t="str">
         <v>General Surgery</v>
@@ -1853,7 +1853,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D73" t="str">
-        <v>11:43:07</v>
+        <v>11:43:09</v>
       </c>
       <c r="E73" t="str">
         <v>Scan</v>
@@ -1864,7 +1864,7 @@
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>190981</v>
+        <v>200163</v>
       </c>
       <c r="B74" t="str">
         <v>General Surgery</v>
@@ -1873,7 +1873,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D74" t="str">
-        <v>11:43:09</v>
+        <v>11:43:12</v>
       </c>
       <c r="E74" t="str">
         <v>Scan</v>
@@ -1884,7 +1884,7 @@
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>200163</v>
+        <v>191061</v>
       </c>
       <c r="B75" t="str">
         <v>General Surgery</v>
@@ -1893,7 +1893,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D75" t="str">
-        <v>11:43:12</v>
+        <v>11:43:15</v>
       </c>
       <c r="E75" t="str">
         <v>Scan</v>
@@ -1904,7 +1904,7 @@
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>191061</v>
+        <v>200744</v>
       </c>
       <c r="B76" t="str">
         <v>General Surgery</v>
@@ -1913,7 +1913,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D76" t="str">
-        <v>11:43:15</v>
+        <v>11:43:17</v>
       </c>
       <c r="E76" t="str">
         <v>Scan</v>
@@ -1924,7 +1924,7 @@
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>200744</v>
+        <v>201564</v>
       </c>
       <c r="B77" t="str">
         <v>General Surgery</v>
@@ -1933,7 +1933,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D77" t="str">
-        <v>11:43:17</v>
+        <v>11:43:20</v>
       </c>
       <c r="E77" t="str">
         <v>Scan</v>
@@ -1944,7 +1944,7 @@
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>201564</v>
+        <v>200804</v>
       </c>
       <c r="B78" t="str">
         <v>General Surgery</v>
@@ -1953,7 +1953,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D78" t="str">
-        <v>11:43:20</v>
+        <v>11:43:22</v>
       </c>
       <c r="E78" t="str">
         <v>Scan</v>
@@ -1964,7 +1964,7 @@
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>200804</v>
+        <v>200792</v>
       </c>
       <c r="B79" t="str">
         <v>General Surgery</v>
@@ -1973,7 +1973,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D79" t="str">
-        <v>11:43:22</v>
+        <v>11:43:24</v>
       </c>
       <c r="E79" t="str">
         <v>Scan</v>
@@ -1984,7 +1984,7 @@
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>200792</v>
+        <v>200628</v>
       </c>
       <c r="B80" t="str">
         <v>General Surgery</v>
@@ -1993,7 +1993,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D80" t="str">
-        <v>11:43:24</v>
+        <v>11:43:26</v>
       </c>
       <c r="E80" t="str">
         <v>Scan</v>
@@ -2004,7 +2004,7 @@
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>200628</v>
+        <v>211216</v>
       </c>
       <c r="B81" t="str">
         <v>General Surgery</v>
@@ -2013,7 +2013,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D81" t="str">
-        <v>11:43:26</v>
+        <v>11:43:28</v>
       </c>
       <c r="E81" t="str">
         <v>Scan</v>
@@ -2024,7 +2024,7 @@
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>211216</v>
+        <v>211197</v>
       </c>
       <c r="B82" t="str">
         <v>General Surgery</v>
@@ -2033,7 +2033,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D82" t="str">
-        <v>11:43:28</v>
+        <v>11:43:31</v>
       </c>
       <c r="E82" t="str">
         <v>Scan</v>
@@ -2044,7 +2044,7 @@
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>211197</v>
+        <v>201397</v>
       </c>
       <c r="B83" t="str">
         <v>General Surgery</v>
@@ -2053,7 +2053,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D83" t="str">
-        <v>11:43:31</v>
+        <v>11:43:33</v>
       </c>
       <c r="E83" t="str">
         <v>Scan</v>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>201397</v>
+        <v>200917</v>
       </c>
       <c r="B84" t="str">
         <v>General Surgery</v>
@@ -2073,7 +2073,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D84" t="str">
-        <v>11:43:33</v>
+        <v>11:43:35</v>
       </c>
       <c r="E84" t="str">
         <v>Scan</v>
@@ -2084,7 +2084,7 @@
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>200917</v>
+        <v>201051</v>
       </c>
       <c r="B85" t="str">
         <v>General Surgery</v>
@@ -2093,7 +2093,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D85" t="str">
-        <v>11:43:35</v>
+        <v>11:43:37</v>
       </c>
       <c r="E85" t="str">
         <v>Scan</v>
@@ -2104,7 +2104,7 @@
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>201051</v>
+        <v>201501</v>
       </c>
       <c r="B86" t="str">
         <v>General Surgery</v>
@@ -2113,7 +2113,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D86" t="str">
-        <v>11:43:37</v>
+        <v>11:43:40</v>
       </c>
       <c r="E86" t="str">
         <v>Scan</v>
@@ -2124,7 +2124,7 @@
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>201501</v>
+        <v>200905</v>
       </c>
       <c r="B87" t="str">
         <v>General Surgery</v>
@@ -2133,7 +2133,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D87" t="str">
-        <v>11:43:40</v>
+        <v>11:43:42</v>
       </c>
       <c r="E87" t="str">
         <v>Scan</v>
@@ -2144,7 +2144,7 @@
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>200905</v>
+        <v>200938</v>
       </c>
       <c r="B88" t="str">
         <v>General Surgery</v>
@@ -2153,7 +2153,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D88" t="str">
-        <v>11:43:42</v>
+        <v>11:43:45</v>
       </c>
       <c r="E88" t="str">
         <v>Scan</v>
@@ -2164,7 +2164,7 @@
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>200938</v>
+        <v>211043</v>
       </c>
       <c r="B89" t="str">
         <v>General Surgery</v>
@@ -2173,7 +2173,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D89" t="str">
-        <v>11:43:45</v>
+        <v>11:43:47</v>
       </c>
       <c r="E89" t="str">
         <v>Scan</v>
@@ -2184,7 +2184,7 @@
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>211043</v>
+        <v>211133</v>
       </c>
       <c r="B90" t="str">
         <v>General Surgery</v>
@@ -2193,7 +2193,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D90" t="str">
-        <v>11:43:47</v>
+        <v>11:43:49</v>
       </c>
       <c r="E90" t="str">
         <v>Scan</v>
@@ -2204,7 +2204,7 @@
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>211133</v>
+        <v>211741</v>
       </c>
       <c r="B91" t="str">
         <v>General Surgery</v>
@@ -2213,7 +2213,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D91" t="str">
-        <v>11:43:49</v>
+        <v>11:43:50</v>
       </c>
       <c r="E91" t="str">
         <v>Scan</v>
@@ -2224,7 +2224,7 @@
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>211741</v>
+        <v>211245</v>
       </c>
       <c r="B92" t="str">
         <v>General Surgery</v>
@@ -2233,7 +2233,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D92" t="str">
-        <v>11:43:50</v>
+        <v>11:43:52</v>
       </c>
       <c r="E92" t="str">
         <v>Scan</v>
@@ -2244,7 +2244,7 @@
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>211245</v>
+        <v>190929</v>
       </c>
       <c r="B93" t="str">
         <v>General Surgery</v>
@@ -2253,7 +2253,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D93" t="str">
-        <v>11:43:52</v>
+        <v>11:43:55</v>
       </c>
       <c r="E93" t="str">
         <v>Scan</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>190929</v>
+        <v>191119</v>
       </c>
       <c r="B94" t="str">
         <v>General Surgery</v>
@@ -2273,7 +2273,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D94" t="str">
-        <v>11:43:55</v>
+        <v>11:43:56</v>
       </c>
       <c r="E94" t="str">
         <v>Scan</v>
@@ -2284,7 +2284,7 @@
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>191119</v>
+        <v>211210</v>
       </c>
       <c r="B95" t="str">
         <v>General Surgery</v>
@@ -2293,10 +2293,10 @@
         <v>11/10/2025</v>
       </c>
       <c r="D95" t="str">
-        <v>11:43:56</v>
+        <v>11:44:43</v>
       </c>
       <c r="E95" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F95" t="str">
         <v>dnasr281@gmail.com</v>
@@ -2304,7 +2304,7 @@
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>211210</v>
+        <v>201880</v>
       </c>
       <c r="B96" t="str">
         <v>General Surgery</v>
@@ -2313,7 +2313,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D96" t="str">
-        <v>11:44:43</v>
+        <v>11:45:28</v>
       </c>
       <c r="E96" t="str">
         <v>Manual</v>
@@ -2324,7 +2324,7 @@
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>201880</v>
+        <v>211246</v>
       </c>
       <c r="B97" t="str">
         <v>General Surgery</v>
@@ -2333,7 +2333,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D97" t="str">
-        <v>11:45:28</v>
+        <v>11:45:59</v>
       </c>
       <c r="E97" t="str">
         <v>Manual</v>
@@ -2344,7 +2344,7 @@
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>211246</v>
+        <v>201823</v>
       </c>
       <c r="B98" t="str">
         <v>General Surgery</v>
@@ -2353,7 +2353,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D98" t="str">
-        <v>11:45:59</v>
+        <v>11:46:33</v>
       </c>
       <c r="E98" t="str">
         <v>Manual</v>
@@ -2364,7 +2364,7 @@
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>201823</v>
+        <v>200928</v>
       </c>
       <c r="B99" t="str">
         <v>General Surgery</v>
@@ -2373,7 +2373,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D99" t="str">
-        <v>11:46:33</v>
+        <v>11:47:11</v>
       </c>
       <c r="E99" t="str">
         <v>Manual</v>
@@ -2384,7 +2384,7 @@
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>200928</v>
+        <v>201237</v>
       </c>
       <c r="B100" t="str">
         <v>General Surgery</v>
@@ -2393,7 +2393,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D100" t="str">
-        <v>11:47:11</v>
+        <v>11:47:35</v>
       </c>
       <c r="E100" t="str">
         <v>Manual</v>
@@ -2404,7 +2404,7 @@
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>201237</v>
+        <v>201513</v>
       </c>
       <c r="B101" t="str">
         <v>General Surgery</v>
@@ -2413,7 +2413,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D101" t="str">
-        <v>11:47:35</v>
+        <v>11:48:02</v>
       </c>
       <c r="E101" t="str">
         <v>Manual</v>
@@ -2424,7 +2424,7 @@
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>201513</v>
+        <v>200997</v>
       </c>
       <c r="B102" t="str">
         <v>General Surgery</v>
@@ -2433,7 +2433,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D102" t="str">
-        <v>11:48:02</v>
+        <v>11:48:26</v>
       </c>
       <c r="E102" t="str">
         <v>Manual</v>
@@ -2444,7 +2444,7 @@
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>200997</v>
+        <v>181004</v>
       </c>
       <c r="B103" t="str">
         <v>General Surgery</v>
@@ -2453,7 +2453,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D103" t="str">
-        <v>11:48:26</v>
+        <v>11:48:49</v>
       </c>
       <c r="E103" t="str">
         <v>Manual</v>
@@ -2464,7 +2464,7 @@
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>181004</v>
+        <v>211121</v>
       </c>
       <c r="B104" t="str">
         <v>General Surgery</v>
@@ -2473,7 +2473,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D104" t="str">
-        <v>11:48:49</v>
+        <v>11:49:14</v>
       </c>
       <c r="E104" t="str">
         <v>Manual</v>
@@ -2484,7 +2484,7 @@
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>211121</v>
+        <v>201252</v>
       </c>
       <c r="B105" t="str">
         <v>General Surgery</v>
@@ -2493,7 +2493,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D105" t="str">
-        <v>11:49:14</v>
+        <v>11:49:29</v>
       </c>
       <c r="E105" t="str">
         <v>Manual</v>
@@ -2504,7 +2504,7 @@
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>201252</v>
+        <v>201023</v>
       </c>
       <c r="B106" t="str">
         <v>General Surgery</v>
@@ -2513,7 +2513,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D106" t="str">
-        <v>11:49:29</v>
+        <v>11:49:42</v>
       </c>
       <c r="E106" t="str">
         <v>Manual</v>
@@ -2524,7 +2524,7 @@
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>201023</v>
+        <v>201253</v>
       </c>
       <c r="B107" t="str">
         <v>General Surgery</v>
@@ -2533,7 +2533,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D107" t="str">
-        <v>11:49:42</v>
+        <v>11:49:57</v>
       </c>
       <c r="E107" t="str">
         <v>Manual</v>
@@ -2544,7 +2544,7 @@
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>201253</v>
+        <v>201337</v>
       </c>
       <c r="B108" t="str">
         <v>General Surgery</v>
@@ -2553,7 +2553,7 @@
         <v>11/10/2025</v>
       </c>
       <c r="D108" t="str">
-        <v>11:49:57</v>
+        <v>11:50:11</v>
       </c>
       <c r="E108" t="str">
         <v>Manual</v>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>201337</v>
+        <v>201572</v>
       </c>
       <c r="B109" t="str">
         <v>General Surgery</v>
@@ -2573,10 +2573,10 @@
         <v>11/10/2025</v>
       </c>
       <c r="D109" t="str">
-        <v>11:50:11</v>
+        <v>11:50:20</v>
       </c>
       <c r="E109" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F109" t="str">
         <v>dnasr281@gmail.com</v>
@@ -2584,7 +2584,7 @@
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>201572</v>
+        <v>201398</v>
       </c>
       <c r="B110" t="str">
         <v>General Surgery</v>
@@ -2593,38 +2593,18 @@
         <v>11/10/2025</v>
       </c>
       <c r="D110" t="str">
-        <v>11:50:20</v>
+        <v>11:50:41</v>
       </c>
       <c r="E110" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F110" t="str">
-        <v>dnasr281@gmail.com</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="str">
-        <v>201398</v>
-      </c>
-      <c r="B111" t="str">
-        <v>General Surgery</v>
-      </c>
-      <c r="C111" t="str">
-        <v>11/10/2025</v>
-      </c>
-      <c r="D111" t="str">
-        <v>11:50:41</v>
-      </c>
-      <c r="E111" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F111" t="str">
         <v>dnasr281@gmail.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F111"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F110"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>